<commit_message>
Revert "Updated Logbook and added Perifericos"
This reverts commit dbdd964fc060a66478d0325b46005da320524534.
</commit_message>
<xml_diff>
--- a/04Code/Perifericos.xlsx
+++ b/04Code/Perifericos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/a88231_uminho_pt/Documents/Documentos/Github/DWR-19/04Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="518" documentId="11_AD4DF034E34935FBC521DC3B6FDD5B1A5BDEDD89" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39A7168C-A75F-41E3-86FA-00BA72A17F67}"/>
+  <xr:revisionPtr revIDLastSave="512" documentId="11_AD4DF034E34935FBC521DC3B6FDD5B1A5BDEDD89" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{942A9362-58AE-4DE3-87E0-8D03C27A00BD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>Porto</t>
   </si>
@@ -204,6 +204,9 @@
     <t>IN 2 - Motor  Direita</t>
   </si>
   <si>
+    <t>USART 1 - RX/  IN motor (Conflito)</t>
+  </si>
+  <si>
     <t>GPIO</t>
   </si>
   <si>
@@ -231,21 +234,6 @@
   <si>
     <t>Resolver Conflito entre USART1  e saída de controlo do
 Motor no pino B15</t>
-  </si>
-  <si>
-    <t>PWM Motor Direita</t>
-  </si>
-  <si>
-    <t>USART 1 - RX/  IN 1 Motor Direita (Conflito)</t>
-  </si>
-  <si>
-    <t>IN 1 - Motor Esquerda</t>
-  </si>
-  <si>
-    <t>IN 2 - Motor  Esquerda</t>
-  </si>
-  <si>
-    <t>PWM Motor Esquerda</t>
   </si>
 </sst>
 </file>
@@ -977,18 +965,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1016,6 +992,132 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1024,141 +1126,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1691,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,7 +1730,7 @@
       </c>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="40" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="3">
@@ -1751,14 +1739,14 @@
       <c r="E10" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="40" t="s">
         <v>6</v>
       </c>
       <c r="H10" s="3">
         <v>0</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="K10" s="52" t="s">
+      <c r="K10" s="48" t="s">
         <v>8</v>
       </c>
       <c r="L10" s="3">
@@ -1767,272 +1755,270 @@
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="45"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="5">
         <v>1</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="G11" s="45"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="7">
         <v>1</v>
       </c>
       <c r="I11" s="6"/>
-      <c r="K11" s="52"/>
+      <c r="K11" s="48"/>
       <c r="L11" s="7">
         <v>1</v>
       </c>
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="45"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="5">
         <v>2</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="G12" s="45"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="7">
         <v>2</v>
       </c>
       <c r="I12" s="6"/>
-      <c r="K12" s="52"/>
+      <c r="K12" s="48"/>
       <c r="L12" s="7">
         <v>2</v>
       </c>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="45"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="7">
         <v>3</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="45"/>
+      <c r="G13" s="41"/>
       <c r="H13" s="7">
         <v>3</v>
       </c>
       <c r="I13" s="6"/>
-      <c r="K13" s="52"/>
+      <c r="K13" s="48"/>
       <c r="L13" s="7">
         <v>3</v>
       </c>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="45"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="7">
         <v>4</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="45"/>
+      <c r="G14" s="41"/>
       <c r="H14" s="7">
         <v>4</v>
       </c>
       <c r="I14" s="6"/>
-      <c r="K14" s="52"/>
+      <c r="K14" s="48"/>
       <c r="L14" s="5">
         <v>4</v>
       </c>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="45"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="7">
         <v>5</v>
       </c>
       <c r="E15" s="21"/>
-      <c r="G15" s="45"/>
+      <c r="G15" s="41"/>
       <c r="H15" s="7">
         <v>5</v>
       </c>
       <c r="I15" s="6"/>
-      <c r="K15" s="52"/>
+      <c r="K15" s="48"/>
       <c r="L15" s="5">
         <v>5</v>
       </c>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="45"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="7">
         <v>6</v>
       </c>
       <c r="E16" s="21"/>
-      <c r="G16" s="45"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="7">
         <v>6</v>
       </c>
       <c r="I16" s="6"/>
-      <c r="K16" s="52"/>
+      <c r="K16" s="48"/>
       <c r="L16" s="5">
         <v>6</v>
       </c>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="45"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="7">
         <v>7</v>
       </c>
       <c r="E17" s="21"/>
-      <c r="G17" s="45"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="7">
         <v>7</v>
       </c>
       <c r="I17" s="6"/>
-      <c r="K17" s="52"/>
+      <c r="K17" s="48"/>
       <c r="L17" s="5">
         <v>7</v>
       </c>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="45"/>
+      <c r="C18" s="41"/>
       <c r="D18" s="5">
         <v>8</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="G18" s="45"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="5">
         <v>8</v>
       </c>
       <c r="I18" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="52"/>
+      <c r="K18" s="48"/>
       <c r="L18" s="5">
         <v>8</v>
       </c>
       <c r="M18" s="6"/>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C19" s="45"/>
+      <c r="C19" s="41"/>
       <c r="D19" s="5">
         <v>9</v>
       </c>
       <c r="E19" s="6"/>
-      <c r="G19" s="45"/>
+      <c r="G19" s="41"/>
       <c r="H19" s="5">
         <v>9</v>
       </c>
       <c r="I19" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K19" s="52"/>
+      <c r="K19" s="48"/>
       <c r="L19" s="7">
         <v>9</v>
       </c>
       <c r="M19" s="6"/>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C20" s="45"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="5">
         <v>10</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="G20" s="45"/>
+      <c r="G20" s="41"/>
       <c r="H20" s="5">
         <v>10</v>
       </c>
       <c r="I20" s="6"/>
-      <c r="K20" s="52"/>
+      <c r="K20" s="48"/>
       <c r="L20" s="5">
         <v>10</v>
       </c>
       <c r="M20" s="6"/>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C21" s="45"/>
+      <c r="C21" s="41"/>
       <c r="D21" s="5">
         <v>11</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="G21" s="45"/>
+      <c r="G21" s="41"/>
       <c r="H21" s="7">
         <v>11</v>
       </c>
       <c r="I21" s="6"/>
-      <c r="K21" s="52"/>
+      <c r="K21" s="48"/>
       <c r="L21" s="5">
         <v>11</v>
       </c>
       <c r="M21" s="6"/>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="45"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="5">
         <v>12</v>
       </c>
       <c r="E22" s="6"/>
-      <c r="G22" s="45"/>
+      <c r="G22" s="41"/>
       <c r="H22" s="7">
         <v>12</v>
       </c>
       <c r="I22" s="6"/>
-      <c r="K22" s="52"/>
+      <c r="K22" s="48"/>
       <c r="L22" s="5">
         <v>12</v>
       </c>
       <c r="M22" s="6"/>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C23" s="45"/>
+      <c r="C23" s="41"/>
       <c r="D23" s="5">
         <v>13</v>
       </c>
       <c r="E23" s="6"/>
-      <c r="G23" s="45"/>
+      <c r="G23" s="41"/>
       <c r="H23" s="7">
         <v>13</v>
       </c>
       <c r="I23" s="6"/>
-      <c r="K23" s="52"/>
+      <c r="K23" s="48"/>
       <c r="L23" s="5">
         <v>13</v>
       </c>
       <c r="M23" s="6"/>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="45"/>
+      <c r="C24" s="41"/>
       <c r="D24" s="5">
         <v>14</v>
       </c>
       <c r="E24" s="6"/>
-      <c r="G24" s="45"/>
+      <c r="G24" s="41"/>
       <c r="H24" s="7">
         <v>14</v>
       </c>
       <c r="I24" s="6"/>
-      <c r="K24" s="52"/>
+      <c r="K24" s="48"/>
       <c r="L24" s="7">
         <v>14</v>
       </c>
       <c r="M24" s="6"/>
     </row>
     <row r="25" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="46"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="8">
         <v>15</v>
       </c>
-      <c r="E25" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="G25" s="46"/>
+      <c r="E25" s="83"/>
+      <c r="G25" s="42"/>
       <c r="H25" s="8">
         <v>15</v>
       </c>
       <c r="I25" s="9"/>
-      <c r="K25" s="48"/>
+      <c r="K25" s="44"/>
       <c r="L25" s="10">
         <v>15</v>
       </c>
       <c r="M25" s="9"/>
     </row>
     <row r="26" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="45" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="3">
@@ -2041,14 +2027,14 @@
       <c r="E26" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="49" t="s">
+      <c r="G26" s="45" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="K26" s="47" t="s">
+      <c r="K26" s="43" t="s">
         <v>9</v>
       </c>
       <c r="L26" s="11">
@@ -2057,233 +2043,231 @@
       <c r="M26" s="4"/>
     </row>
     <row r="27" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="50"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="7">
         <v>1</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="50"/>
+      <c r="G27" s="46"/>
       <c r="H27" s="5">
         <v>1</v>
       </c>
       <c r="I27" s="6"/>
-      <c r="K27" s="48"/>
+      <c r="K27" s="44"/>
       <c r="L27" s="12">
         <v>1</v>
       </c>
       <c r="M27" s="13"/>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C28" s="50"/>
+      <c r="C28" s="46"/>
       <c r="D28" s="7">
         <v>2</v>
       </c>
       <c r="E28" s="6"/>
-      <c r="G28" s="50"/>
+      <c r="G28" s="46"/>
       <c r="H28" s="7">
         <v>2</v>
       </c>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C29" s="50"/>
+      <c r="C29" s="46"/>
       <c r="D29" s="5">
         <v>3</v>
       </c>
       <c r="E29" s="6"/>
-      <c r="G29" s="50"/>
+      <c r="G29" s="46"/>
       <c r="H29" s="7">
         <v>3</v>
       </c>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="50"/>
+      <c r="C30" s="46"/>
       <c r="D30" s="7">
         <v>4</v>
       </c>
       <c r="E30" s="6"/>
-      <c r="G30" s="50"/>
+      <c r="G30" s="46"/>
       <c r="H30" s="7">
         <v>4</v>
       </c>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C31" s="50"/>
+      <c r="C31" s="46"/>
       <c r="D31" s="7">
         <v>5</v>
       </c>
       <c r="E31" s="6"/>
-      <c r="G31" s="50"/>
+      <c r="G31" s="46"/>
       <c r="H31" s="7">
         <v>5</v>
       </c>
       <c r="I31" s="6"/>
-      <c r="K31" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="L31" s="54"/>
-      <c r="M31" s="55"/>
+      <c r="K31" s="91" t="s">
+        <v>57</v>
+      </c>
+      <c r="L31" s="92"/>
+      <c r="M31" s="93"/>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C32" s="50"/>
+      <c r="C32" s="46"/>
       <c r="D32" s="7">
         <v>6</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="50"/>
+      <c r="G32" s="46"/>
       <c r="H32" s="7">
         <v>6</v>
       </c>
       <c r="I32" s="6"/>
-      <c r="K32" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="L32" s="57"/>
-      <c r="M32" s="58"/>
+      <c r="K32" s="100" t="s">
+        <v>58</v>
+      </c>
+      <c r="L32" s="95"/>
+      <c r="M32" s="96"/>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C33" s="50"/>
+      <c r="C33" s="46"/>
       <c r="D33" s="5">
         <v>7</v>
       </c>
       <c r="E33" s="6"/>
-      <c r="G33" s="50"/>
+      <c r="G33" s="46"/>
       <c r="H33" s="7">
         <v>7</v>
       </c>
       <c r="I33" s="6"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="58"/>
+      <c r="K33" s="94"/>
+      <c r="L33" s="95"/>
+      <c r="M33" s="96"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C34" s="50"/>
+      <c r="C34" s="46"/>
       <c r="D34" s="7">
         <v>8</v>
       </c>
       <c r="E34" s="6"/>
-      <c r="G34" s="50"/>
+      <c r="G34" s="46"/>
       <c r="H34" s="7">
         <v>8</v>
       </c>
       <c r="I34" s="6"/>
-      <c r="K34" s="59"/>
-      <c r="L34" s="57"/>
-      <c r="M34" s="58"/>
+      <c r="K34" s="94"/>
+      <c r="L34" s="95"/>
+      <c r="M34" s="96"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C35" s="50"/>
+      <c r="C35" s="46"/>
       <c r="D35" s="7">
         <v>9</v>
       </c>
       <c r="E35" s="6"/>
-      <c r="G35" s="50"/>
+      <c r="G35" s="46"/>
       <c r="H35" s="7">
         <v>9</v>
       </c>
       <c r="I35" s="6"/>
-      <c r="K35" s="59"/>
-      <c r="L35" s="57"/>
-      <c r="M35" s="58"/>
+      <c r="K35" s="94"/>
+      <c r="L35" s="95"/>
+      <c r="M35" s="96"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C36" s="50"/>
+      <c r="C36" s="46"/>
       <c r="D36" s="7">
         <v>10</v>
       </c>
       <c r="E36" s="6"/>
-      <c r="G36" s="50"/>
+      <c r="G36" s="46"/>
       <c r="H36" s="7">
         <v>10</v>
       </c>
       <c r="I36" s="6"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="57"/>
-      <c r="M36" s="58"/>
+      <c r="K36" s="94"/>
+      <c r="L36" s="95"/>
+      <c r="M36" s="96"/>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C37" s="50"/>
+      <c r="C37" s="46"/>
       <c r="D37" s="7">
         <v>11</v>
       </c>
       <c r="E37" s="6"/>
-      <c r="G37" s="50"/>
+      <c r="G37" s="46"/>
       <c r="H37" s="7">
         <v>11</v>
       </c>
       <c r="I37" s="6"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="57"/>
-      <c r="M37" s="58"/>
+      <c r="K37" s="94"/>
+      <c r="L37" s="95"/>
+      <c r="M37" s="96"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C38" s="50"/>
+      <c r="C38" s="46"/>
       <c r="D38" s="7">
         <v>12</v>
       </c>
-      <c r="E38" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="G38" s="50"/>
+      <c r="E38" s="82"/>
+      <c r="G38" s="46"/>
       <c r="H38" s="7">
         <v>12</v>
       </c>
       <c r="I38" s="6"/>
-      <c r="K38" s="59"/>
-      <c r="L38" s="57"/>
-      <c r="M38" s="58"/>
+      <c r="K38" s="94"/>
+      <c r="L38" s="95"/>
+      <c r="M38" s="96"/>
     </row>
     <row r="39" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="50"/>
+      <c r="C39" s="46"/>
       <c r="D39" s="7">
         <v>13</v>
       </c>
-      <c r="E39" s="40" t="s">
+      <c r="E39" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="G39" s="50"/>
+      <c r="G39" s="46"/>
       <c r="H39" s="7">
         <v>13</v>
       </c>
       <c r="I39" s="6"/>
-      <c r="K39" s="60"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="62"/>
+      <c r="K39" s="97"/>
+      <c r="L39" s="98"/>
+      <c r="M39" s="99"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C40" s="50"/>
+      <c r="C40" s="46"/>
       <c r="D40" s="5">
         <v>14</v>
       </c>
       <c r="E40" s="6"/>
-      <c r="G40" s="50"/>
+      <c r="G40" s="46"/>
       <c r="H40" s="7">
         <v>14</v>
       </c>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="51"/>
+      <c r="C41" s="47"/>
       <c r="D41" s="8">
         <v>15</v>
       </c>
-      <c r="E41" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="G41" s="51"/>
+      <c r="E41" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="G41" s="47"/>
       <c r="H41" s="8">
         <v>15</v>
       </c>
       <c r="I41" s="9"/>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="40" t="s">
         <v>4</v>
       </c>
       <c r="D42" s="3">
@@ -2292,7 +2276,7 @@
       <c r="E42" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="G42" s="44" t="s">
+      <c r="G42" s="40" t="s">
         <v>7</v>
       </c>
       <c r="H42" s="3">
@@ -2301,194 +2285,190 @@
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C43" s="45"/>
+      <c r="C43" s="41"/>
       <c r="D43" s="5">
         <v>1</v>
       </c>
       <c r="E43" s="6"/>
-      <c r="G43" s="45"/>
+      <c r="G43" s="41"/>
       <c r="H43" s="7">
         <v>1</v>
       </c>
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C44" s="45"/>
+      <c r="C44" s="41"/>
       <c r="D44" s="7">
         <v>2</v>
       </c>
       <c r="E44" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G44" s="45"/>
+      <c r="G44" s="41"/>
       <c r="H44" s="7">
         <v>2</v>
       </c>
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C45" s="45"/>
+      <c r="C45" s="41"/>
       <c r="D45" s="7">
         <v>3</v>
       </c>
       <c r="E45" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G45" s="45"/>
+      <c r="G45" s="41"/>
       <c r="H45" s="7">
         <v>3</v>
       </c>
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C46" s="45"/>
+      <c r="C46" s="41"/>
       <c r="D46" s="5">
         <v>4</v>
       </c>
       <c r="E46" s="6"/>
-      <c r="G46" s="45"/>
+      <c r="G46" s="41"/>
       <c r="H46" s="7">
         <v>4</v>
       </c>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C47" s="45"/>
+      <c r="C47" s="41"/>
       <c r="D47" s="5">
         <v>5</v>
       </c>
       <c r="E47" s="6"/>
-      <c r="G47" s="45"/>
+      <c r="G47" s="41"/>
       <c r="H47" s="7">
         <v>5</v>
       </c>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C48" s="45"/>
+      <c r="C48" s="41"/>
       <c r="D48" s="7">
         <v>6</v>
       </c>
-      <c r="E48" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="G48" s="45"/>
+      <c r="E48" s="82"/>
+      <c r="G48" s="41"/>
       <c r="H48" s="5">
         <v>6</v>
       </c>
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C49" s="45"/>
+      <c r="C49" s="41"/>
       <c r="D49" s="7">
         <v>7</v>
       </c>
-      <c r="E49" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="G49" s="45"/>
+      <c r="E49" s="82"/>
+      <c r="G49" s="41"/>
       <c r="H49" s="7">
         <v>7</v>
       </c>
       <c r="I49" s="6"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="45"/>
+      <c r="C50" s="41"/>
       <c r="D50" s="7">
         <v>8</v>
       </c>
       <c r="E50" s="6"/>
-      <c r="G50" s="45"/>
+      <c r="G50" s="41"/>
       <c r="H50" s="7">
         <v>8</v>
       </c>
       <c r="I50" s="6"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C51" s="45"/>
+      <c r="C51" s="41"/>
       <c r="D51" s="7">
         <v>9</v>
       </c>
       <c r="E51" s="6"/>
-      <c r="G51" s="45"/>
+      <c r="G51" s="41"/>
       <c r="H51" s="7">
         <v>9</v>
       </c>
       <c r="I51" s="6"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C52" s="45"/>
+      <c r="C52" s="41"/>
       <c r="D52" s="7">
         <v>10</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G52" s="45"/>
+      <c r="G52" s="41"/>
       <c r="H52" s="7">
         <v>10</v>
       </c>
       <c r="I52" s="6"/>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C53" s="45"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="7">
         <v>11</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G53" s="45"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="5">
         <v>11</v>
       </c>
       <c r="I53" s="6"/>
     </row>
     <row r="54" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="45"/>
+      <c r="C54" s="41"/>
       <c r="D54" s="7">
         <v>12</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G54" s="45"/>
+      <c r="G54" s="41"/>
       <c r="H54" s="7">
         <v>12</v>
       </c>
       <c r="I54" s="6"/>
     </row>
     <row r="55" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="45"/>
+      <c r="C55" s="41"/>
       <c r="D55" s="5">
         <v>13</v>
       </c>
       <c r="E55" s="6"/>
-      <c r="G55" s="45"/>
+      <c r="G55" s="41"/>
       <c r="H55" s="7">
         <v>13</v>
       </c>
       <c r="I55" s="6"/>
     </row>
     <row r="56" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="45"/>
+      <c r="C56" s="41"/>
       <c r="D56" s="5">
         <v>14</v>
       </c>
       <c r="E56" s="6"/>
-      <c r="G56" s="45"/>
+      <c r="G56" s="41"/>
       <c r="H56" s="7">
         <v>14</v>
       </c>
       <c r="I56" s="6"/>
     </row>
     <row r="57" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="46"/>
+      <c r="C57" s="42"/>
       <c r="D57" s="10">
         <v>15</v>
       </c>
       <c r="E57" s="9"/>
-      <c r="G57" s="46"/>
+      <c r="G57" s="42"/>
       <c r="H57" s="8">
         <v>15</v>
       </c>
@@ -2528,32 +2508,32 @@
   <sheetData>
     <row r="3" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="81"/>
-      <c r="H4" s="82" t="s">
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="78"/>
+      <c r="H4" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="83"/>
-      <c r="J4" s="84"/>
-      <c r="L4" s="71" t="s">
+      <c r="I4" s="80"/>
+      <c r="J4" s="81"/>
+      <c r="L4" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="72"/>
-      <c r="N4" s="73"/>
-      <c r="P4" s="71" t="s">
+      <c r="M4" s="69"/>
+      <c r="N4" s="70"/>
+      <c r="P4" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="73"/>
-      <c r="T4" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="U4" s="72"/>
-      <c r="V4" s="73"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="70"/>
+      <c r="T4" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="69"/>
+      <c r="V4" s="70"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="31" t="s">
@@ -2606,7 +2586,7 @@
       </c>
     </row>
     <row r="6" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="73" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="22">
@@ -2618,7 +2598,7 @@
       <c r="F6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="76" t="s">
+      <c r="H6" s="73" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="26">
@@ -2627,7 +2607,7 @@
       <c r="J6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="85" t="s">
+      <c r="L6" s="71" t="s">
         <v>3</v>
       </c>
       <c r="M6" s="22">
@@ -2636,7 +2616,7 @@
       <c r="N6" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="45" t="s">
+      <c r="P6" s="41" t="s">
         <v>6</v>
       </c>
       <c r="Q6" s="25">
@@ -2648,13 +2628,13 @@
       <c r="T6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="U6" s="43">
+      <c r="U6" s="85">
         <v>15</v>
       </c>
       <c r="V6" s="6"/>
     </row>
     <row r="7" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="77"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="22">
         <v>3</v>
       </c>
@@ -2664,28 +2644,28 @@
       <c r="F7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="77"/>
+      <c r="H7" s="74"/>
       <c r="I7" s="22">
         <v>11</v>
       </c>
       <c r="J7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="86"/>
+      <c r="L7" s="72"/>
       <c r="M7" s="24">
         <v>15</v>
       </c>
       <c r="N7" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="46"/>
+      <c r="P7" s="42"/>
       <c r="Q7" s="12">
         <v>9</v>
       </c>
       <c r="R7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="T7" s="74" t="s">
+      <c r="T7" s="86" t="s">
         <v>3</v>
       </c>
       <c r="U7" s="26">
@@ -2694,7 +2674,7 @@
       <c r="V7" s="29"/>
     </row>
     <row r="8" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="85"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="22">
         <v>4</v>
       </c>
@@ -2704,31 +2684,31 @@
       <c r="F8" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="78"/>
+      <c r="H8" s="75"/>
       <c r="I8" s="24">
         <v>12</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="87" t="s">
+      <c r="L8" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="M8" s="88"/>
-      <c r="N8" s="89"/>
-      <c r="P8" s="87" t="s">
+      <c r="M8" s="55"/>
+      <c r="N8" s="56"/>
+      <c r="P8" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="89"/>
-      <c r="T8" s="52"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="56"/>
+      <c r="T8" s="48"/>
       <c r="U8" s="34">
         <v>13</v>
       </c>
       <c r="V8" s="35"/>
     </row>
     <row r="9" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="74" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="25">
@@ -2740,29 +2720,29 @@
       <c r="F9" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="90" t="s">
+      <c r="H9" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="91"/>
-      <c r="J9" s="92"/>
-      <c r="L9" s="66" t="s">
+      <c r="I9" s="58"/>
+      <c r="J9" s="59"/>
+      <c r="L9" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="67"/>
-      <c r="N9" s="68"/>
-      <c r="P9" s="66" t="s">
+      <c r="M9" s="50"/>
+      <c r="N9" s="51"/>
+      <c r="P9" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="Q9" s="67"/>
-      <c r="R9" s="68"/>
-      <c r="T9" s="75"/>
+      <c r="Q9" s="50"/>
+      <c r="R9" s="51"/>
+      <c r="T9" s="87"/>
       <c r="U9" s="27">
         <v>15</v>
       </c>
       <c r="V9" s="33"/>
     </row>
     <row r="10" spans="3:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="77"/>
+      <c r="C10" s="74"/>
       <c r="D10" s="28">
         <v>9</v>
       </c>
@@ -2772,18 +2752,18 @@
       <c r="F10" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="93" t="s">
+      <c r="H10" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="94"/>
-      <c r="J10" s="95"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="68"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="68"/>
-      <c r="T10" s="74" t="s">
+      <c r="I10" s="61"/>
+      <c r="J10" s="62"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="51"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="51"/>
+      <c r="T10" s="86" t="s">
         <v>4</v>
       </c>
       <c r="U10" s="26">
@@ -2792,7 +2772,7 @@
       <c r="V10" s="29"/>
     </row>
     <row r="11" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="73" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="22">
@@ -2804,23 +2784,23 @@
       <c r="F11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="66"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="97"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="68"/>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="67"/>
-      <c r="R11" s="68"/>
-      <c r="T11" s="48"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="64"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="51"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="51"/>
+      <c r="T11" s="44"/>
       <c r="U11" s="36">
         <v>7</v>
       </c>
       <c r="V11" s="37"/>
     </row>
     <row r="12" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C12" s="77"/>
+      <c r="C12" s="74"/>
       <c r="D12" s="22">
         <v>12</v>
       </c>
@@ -2830,18 +2810,18 @@
       <c r="F12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="66"/>
-      <c r="I12" s="96"/>
-      <c r="J12" s="97"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="68"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="67"/>
-      <c r="R12" s="68"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="64"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="51"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="51"/>
     </row>
     <row r="13" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="78"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="24">
         <v>13</v>
       </c>
@@ -2851,162 +2831,151 @@
       <c r="F13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="66"/>
-      <c r="I13" s="96"/>
-      <c r="J13" s="97"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="68"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="67"/>
-      <c r="R13" s="68"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="64"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="51"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="51"/>
     </row>
     <row r="14" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C14" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="65"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="97"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="67"/>
-      <c r="N14" s="68"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="67"/>
-      <c r="R14" s="68"/>
+      <c r="C14" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="90"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="64"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="51"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="51"/>
     </row>
     <row r="15" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="51"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="64"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="51"/>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="51"/>
+    </row>
+    <row r="16" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="44"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="53"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="64"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="53"/>
+      <c r="P16" s="44"/>
+      <c r="Q16" s="52"/>
+      <c r="R16" s="53"/>
+    </row>
+    <row r="17" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H17" s="49"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="64"/>
+      <c r="L17" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="M17" s="89"/>
+      <c r="N17" s="90"/>
+      <c r="P17" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="89"/>
+      <c r="R17" s="90"/>
+    </row>
+    <row r="18" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H18" s="49"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="64"/>
+      <c r="L18" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="50"/>
+      <c r="N18" s="51"/>
+      <c r="P18" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="51"/>
+    </row>
+    <row r="19" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="65"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="67"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="51"/>
+      <c r="P19" s="44"/>
+      <c r="Q19" s="52"/>
+      <c r="R19" s="53"/>
+    </row>
+    <row r="20" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H20" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="89"/>
+      <c r="J20" s="90"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="51"/>
+    </row>
+    <row r="21" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H21" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="68"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="96"/>
-      <c r="J15" s="97"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="68"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="67"/>
-      <c r="R15" s="68"/>
-    </row>
-    <row r="16" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="48"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="70"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="96"/>
-      <c r="J16" s="97"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="70"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="69"/>
-      <c r="R16" s="70"/>
-    </row>
-    <row r="17" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H17" s="66"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="97"/>
-      <c r="L17" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="M17" s="64"/>
-      <c r="N17" s="65"/>
-      <c r="P17" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q17" s="64"/>
-      <c r="R17" s="65"/>
-    </row>
-    <row r="18" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H18" s="66"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="97"/>
-      <c r="L18" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="M18" s="67"/>
-      <c r="N18" s="68"/>
-      <c r="P18" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q18" s="67"/>
-      <c r="R18" s="68"/>
-    </row>
-    <row r="19" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H19" s="98"/>
-      <c r="I19" s="99"/>
-      <c r="J19" s="100"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="67"/>
-      <c r="N19" s="68"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="69"/>
-      <c r="R19" s="70"/>
-    </row>
-    <row r="20" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H20" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" s="64"/>
-      <c r="J20" s="65"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="67"/>
-      <c r="N20" s="68"/>
-    </row>
-    <row r="21" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H21" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="I21" s="67"/>
-      <c r="J21" s="68"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="67"/>
-      <c r="N21" s="68"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="51"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="51"/>
     </row>
     <row r="22" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H22" s="52"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="68"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="69"/>
-      <c r="N22" s="70"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="51"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="53"/>
     </row>
     <row r="23" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H23" s="52"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="68"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="51"/>
     </row>
     <row r="24" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H24" s="52"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="68"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="51"/>
     </row>
     <row r="25" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H25" s="48"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="70"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="L9:N16"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R16"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J19"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L18:N22"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J25"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C15:F16"/>
     <mergeCell ref="T4:V4"/>
@@ -3023,6 +2992,17 @@
     <mergeCell ref="P6:P7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N16"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R16"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J19"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="L18:N22"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edit pinout excel, add pinout kicad
</commit_message>
<xml_diff>
--- a/04Code/Perifericos.xlsx
+++ b/04Code/Perifericos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DWR-19\04Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\3ano\2semestre\LPI II\DWR-19\04Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87917838-C57C-4FCF-85B4-AECFBD2C5031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68DE7DB-B48A-4843-A519-F34CDCF354C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinos Usados" sheetId="1" r:id="rId1"/>
@@ -878,12 +878,6 @@
     <t>IN2 Left</t>
   </si>
   <si>
-    <t>PWM RIGHT</t>
-  </si>
-  <si>
-    <t>PWM LEFT</t>
-  </si>
-  <si>
     <t>USART 1 - RX</t>
   </si>
   <si>
@@ -924,6 +918,12 @@
   </si>
   <si>
     <t>PWM - Motor Esquerda</t>
+  </si>
+  <si>
+    <t>PWM Right</t>
+  </si>
+  <si>
+    <t>PWM Left</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1889,15 +1889,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1913,54 +1904,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2001,6 +1944,73 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2285,8 +2295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:AW88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2466,7 +2476,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="50" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G16" s="69"/>
       <c r="H16" s="7">
@@ -2485,7 +2495,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="50" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G17" s="69"/>
       <c r="H17" s="7">
@@ -2632,7 +2642,7 @@
         <v>15</v>
       </c>
       <c r="I25" s="40" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="K25" s="72"/>
       <c r="L25" s="10">
@@ -2771,7 +2781,7 @@
         <v>8</v>
       </c>
       <c r="E34" s="40" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G34" s="74"/>
       <c r="H34" s="7">
@@ -2788,7 +2798,7 @@
         <v>9</v>
       </c>
       <c r="E35" s="40" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G35" s="74"/>
       <c r="H35" s="7">
@@ -2879,7 +2889,7 @@
         <v>15</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G41" s="75"/>
       <c r="H41" s="8">
@@ -2918,7 +2928,7 @@
         <v>1</v>
       </c>
       <c r="I43" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="3:13" x14ac:dyDescent="0.25">
@@ -3058,7 +3068,7 @@
         <v>12</v>
       </c>
       <c r="I54" s="40" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="55" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3072,7 +3082,7 @@
         <v>13</v>
       </c>
       <c r="I55" s="49" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="56" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3150,10 +3160,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D1835F-16BF-4BB4-AE8E-49185A3BFF21}">
-  <dimension ref="C4:AH33"/>
+  <dimension ref="A4:AH33"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AK28" sqref="AK28"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3164,9 +3174,9 @@
     <col min="34" max="34" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="87" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D4" s="88"/>
       <c r="E4" s="88"/>
@@ -3183,7 +3193,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="91" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S4" s="92"/>
       <c r="T4" s="92"/>
@@ -3202,7 +3212,7 @@
       <c r="AG4" s="92"/>
       <c r="AH4" s="92"/>
     </row>
-    <row r="5" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="61"/>
       <c r="D5" s="52"/>
       <c r="E5" s="52"/>
@@ -3226,7 +3236,9 @@
       <c r="O5" s="57"/>
       <c r="P5" s="42"/>
       <c r="Q5" s="42"/>
-      <c r="R5" s="57"/>
+      <c r="R5" s="57" t="s">
+        <v>277</v>
+      </c>
       <c r="S5" s="56"/>
       <c r="T5" s="56"/>
       <c r="U5" s="56"/>
@@ -3244,7 +3256,7 @@
       <c r="AA5" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="AB5" s="56" t="s">
+      <c r="AB5" s="55" t="s">
         <v>161</v>
       </c>
       <c r="AC5" s="56" t="s">
@@ -3259,10 +3271,10 @@
       <c r="AF5" s="56"/>
       <c r="AG5" s="56"/>
       <c r="AH5" s="57" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="6" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="61"/>
       <c r="D6" s="52"/>
       <c r="E6" s="52"/>
@@ -3316,7 +3328,7 @@
       <c r="AA6" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="AB6" s="52" t="s">
+      <c r="AB6" s="46" t="s">
         <v>162</v>
       </c>
       <c r="AC6" s="52" t="s">
@@ -3333,10 +3345,10 @@
       </c>
       <c r="AG6" s="52"/>
       <c r="AH6" s="61" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="61"/>
       <c r="D7" s="52"/>
       <c r="E7" s="52"/>
@@ -3400,7 +3412,7 @@
       <c r="AG7" s="52"/>
       <c r="AH7" s="61"/>
     </row>
-    <row r="8" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="61"/>
       <c r="D8" s="52"/>
       <c r="E8" s="52"/>
@@ -3458,7 +3470,7 @@
       <c r="AG8" s="52"/>
       <c r="AH8" s="61"/>
     </row>
-    <row r="9" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="61"/>
       <c r="D9" s="52"/>
       <c r="E9" s="52"/>
@@ -3524,9 +3536,11 @@
       <c r="AG9" s="52" t="s">
         <v>259</v>
       </c>
-      <c r="AH9" s="61"/>
-    </row>
-    <row r="10" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH9" s="61" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="61"/>
       <c r="D10" s="52"/>
       <c r="E10" s="52"/>
@@ -3566,7 +3580,7 @@
       <c r="AA10" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="AB10" s="55" t="s">
+      <c r="AB10" s="135" t="s">
         <v>176</v>
       </c>
       <c r="AC10" s="52" t="s">
@@ -3579,10 +3593,10 @@
       <c r="AF10" s="52"/>
       <c r="AG10" s="52"/>
       <c r="AH10" s="61" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="11" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="61"/>
       <c r="D11" s="52"/>
       <c r="E11" s="52"/>
@@ -3626,7 +3640,7 @@
       <c r="AA11" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="AB11" s="55" t="s">
+      <c r="AB11" s="135" t="s">
         <v>198</v>
       </c>
       <c r="AC11" s="52" t="s">
@@ -3638,11 +3652,9 @@
       </c>
       <c r="AF11" s="52"/>
       <c r="AG11" s="52"/>
-      <c r="AH11" s="61" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="12" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH11" s="61"/>
+    </row>
+    <row r="12" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="57"/>
       <c r="D12" s="56"/>
       <c r="E12" s="56"/>
@@ -3694,9 +3706,11 @@
       <c r="AE12" s="52"/>
       <c r="AF12" s="52"/>
       <c r="AG12" s="52"/>
-      <c r="AH12" s="61"/>
-    </row>
-    <row r="13" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH12" s="61" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="43"/>
       <c r="D13" s="43"/>
       <c r="E13" s="43"/>
@@ -3734,7 +3748,7 @@
       <c r="AA13" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="AB13" s="52" t="s">
+      <c r="AB13" s="55" t="s">
         <v>162</v>
       </c>
       <c r="AC13" s="52" t="s">
@@ -3745,12 +3759,14 @@
       <c r="AF13" s="52"/>
       <c r="AG13" s="52"/>
       <c r="AH13" s="61" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="14" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="131"/>
+      <c r="B14" s="131"/>
       <c r="C14" s="57" t="s">
-        <v>27</v>
+        <v>276</v>
       </c>
       <c r="D14" s="53" t="s">
         <v>141</v>
@@ -3804,24 +3820,24 @@
       <c r="AA14" s="64" t="s">
         <v>158</v>
       </c>
-      <c r="AB14" s="52"/>
+      <c r="AB14" s="46"/>
       <c r="AC14" s="52"/>
       <c r="AD14" s="52"/>
       <c r="AE14" s="52"/>
       <c r="AF14" s="52"/>
       <c r="AG14" s="52"/>
-      <c r="AH14" s="60" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="15" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH14" s="60"/>
+    </row>
+    <row r="15" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="131"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="57" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D15" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="E15" s="55" t="s">
+      <c r="E15" s="136" t="s">
         <v>135</v>
       </c>
       <c r="F15" s="52"/>
@@ -3862,9 +3878,11 @@
       <c r="AG15" s="44"/>
       <c r="AH15" s="44"/>
     </row>
-    <row r="16" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="131"/>
+      <c r="B16" s="131"/>
       <c r="C16" s="57" t="s">
-        <v>278</v>
+        <v>27</v>
       </c>
       <c r="D16" s="56" t="s">
         <v>142</v>
@@ -3912,12 +3930,12 @@
       <c r="AE16" s="53"/>
       <c r="AF16" s="53"/>
       <c r="AG16" s="53"/>
-      <c r="AH16" s="62" t="s">
-        <v>279</v>
-      </c>
+      <c r="AH16" s="62"/>
     </row>
     <row r="17" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="57"/>
+      <c r="C17" s="57" t="s">
+        <v>28</v>
+      </c>
       <c r="D17" s="56"/>
       <c r="E17" s="46" t="s">
         <v>143</v>
@@ -3967,7 +3985,9 @@
       <c r="AH17" s="57"/>
     </row>
     <row r="18" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="57"/>
+      <c r="C18" s="57" t="s">
+        <v>29</v>
+      </c>
       <c r="D18" s="56"/>
       <c r="E18" s="52" t="s">
         <v>144</v>
@@ -4019,7 +4039,7 @@
       <c r="AH18" s="57"/>
     </row>
     <row r="19" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="57"/>
+      <c r="C19" s="133"/>
       <c r="D19" s="56" t="s">
         <v>146</v>
       </c>
@@ -4072,8 +4092,8 @@
       <c r="AG19" s="56"/>
       <c r="AH19" s="57"/>
     </row>
-    <row r="20" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="57"/>
+    <row r="20" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="132"/>
       <c r="D20" s="56"/>
       <c r="E20" s="52"/>
       <c r="F20" s="52"/>
@@ -4129,9 +4149,11 @@
       <c r="AH20" s="57"/>
     </row>
     <row r="21" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="57"/>
+      <c r="C21" s="57" t="s">
+        <v>30</v>
+      </c>
       <c r="D21" s="56"/>
-      <c r="E21" s="52" t="s">
+      <c r="E21" s="55" t="s">
         <v>136</v>
       </c>
       <c r="F21" s="52" t="s">
@@ -4183,9 +4205,11 @@
       <c r="AH21" s="57"/>
     </row>
     <row r="22" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="57"/>
+      <c r="C22" s="61" t="s">
+        <v>32</v>
+      </c>
       <c r="D22" s="56"/>
-      <c r="E22" s="52"/>
+      <c r="E22" s="46"/>
       <c r="F22" s="52"/>
       <c r="G22" s="52"/>
       <c r="H22" s="51" t="s">
@@ -4245,9 +4269,7 @@
       <c r="AH22" s="57"/>
     </row>
     <row r="23" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="57" t="s">
-        <v>25</v>
-      </c>
+      <c r="C23" s="133"/>
       <c r="D23" s="56"/>
       <c r="E23" s="56" t="s">
         <v>149</v>
@@ -4303,9 +4325,7 @@
       <c r="AH23" s="57"/>
     </row>
     <row r="24" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="57" t="s">
-        <v>28</v>
-      </c>
+      <c r="C24" s="134"/>
       <c r="D24" s="56"/>
       <c r="E24" s="56" t="s">
         <v>150</v>
@@ -4353,7 +4373,7 @@
       <c r="AH24" s="57"/>
     </row>
     <row r="25" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="57"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="56"/>
       <c r="E25" s="56"/>
       <c r="F25" s="56"/>
@@ -4413,9 +4433,7 @@
       <c r="AH25" s="57"/>
     </row>
     <row r="26" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="57" t="s">
-        <v>29</v>
-      </c>
+      <c r="C26" s="134"/>
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
       <c r="F26" s="56" t="s">
@@ -4477,9 +4495,7 @@
       <c r="AH26" s="57"/>
     </row>
     <row r="27" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="57" t="s">
-        <v>32</v>
-      </c>
+      <c r="C27" s="132"/>
       <c r="D27" s="56"/>
       <c r="E27" s="56"/>
       <c r="F27" s="56" t="s">
@@ -4594,7 +4610,7 @@
     </row>
     <row r="29" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="89" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D29" s="90"/>
       <c r="E29" s="90"/>
@@ -4801,7 +4817,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="89" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="S33" s="90"/>
       <c r="T33" s="90"/>
@@ -4837,7 +4853,7 @@
   <dimension ref="C3:V25"/>
   <sheetViews>
     <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J6" sqref="J6:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4847,32 +4863,32 @@
   <sheetData>
     <row r="3" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="109" t="s">
+      <c r="C4" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="111"/>
-      <c r="H4" s="112" t="s">
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="125"/>
+      <c r="H4" s="126" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="113"/>
-      <c r="J4" s="114"/>
-      <c r="L4" s="101" t="s">
+      <c r="I4" s="127"/>
+      <c r="J4" s="128"/>
+      <c r="L4" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="102"/>
-      <c r="N4" s="103"/>
-      <c r="P4" s="101" t="s">
+      <c r="M4" s="116"/>
+      <c r="N4" s="117"/>
+      <c r="P4" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="103"/>
-      <c r="T4" s="101" t="s">
+      <c r="Q4" s="116"/>
+      <c r="R4" s="117"/>
+      <c r="T4" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="U4" s="102"/>
-      <c r="V4" s="103"/>
+      <c r="U4" s="116"/>
+      <c r="V4" s="117"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="31" t="s">
@@ -4925,7 +4941,7 @@
       </c>
     </row>
     <row r="6" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C6" s="106" t="s">
+      <c r="C6" s="120" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="22">
@@ -4937,7 +4953,7 @@
       <c r="F6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="106" t="s">
+      <c r="H6" s="120" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="26">
@@ -4946,7 +4962,7 @@
       <c r="J6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="115" t="s">
+      <c r="L6" s="129" t="s">
         <v>3</v>
       </c>
       <c r="M6" s="22">
@@ -4973,7 +4989,7 @@
       <c r="V6" s="6"/>
     </row>
     <row r="7" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="107"/>
+      <c r="C7" s="121"/>
       <c r="D7" s="22">
         <v>3</v>
       </c>
@@ -4983,14 +4999,14 @@
       <c r="F7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="107"/>
+      <c r="H7" s="121"/>
       <c r="I7" s="22">
         <v>11</v>
       </c>
       <c r="J7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="116"/>
+      <c r="L7" s="130"/>
       <c r="M7" s="24">
         <v>15</v>
       </c>
@@ -5004,7 +5020,7 @@
       <c r="R7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="T7" s="104" t="s">
+      <c r="T7" s="118" t="s">
         <v>3</v>
       </c>
       <c r="U7" s="26">
@@ -5013,7 +5029,7 @@
       <c r="V7" s="29"/>
     </row>
     <row r="8" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="115"/>
+      <c r="C8" s="129"/>
       <c r="D8" s="22">
         <v>4</v>
       </c>
@@ -5023,23 +5039,23 @@
       <c r="F8" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="108"/>
+      <c r="H8" s="122"/>
       <c r="I8" s="24">
         <v>12</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="117" t="s">
+      <c r="L8" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="M8" s="118"/>
-      <c r="N8" s="119"/>
-      <c r="P8" s="117" t="s">
+      <c r="M8" s="99"/>
+      <c r="N8" s="100"/>
+      <c r="P8" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="118"/>
-      <c r="R8" s="119"/>
+      <c r="Q8" s="99"/>
+      <c r="R8" s="100"/>
       <c r="T8" s="76"/>
       <c r="U8" s="34">
         <v>13</v>
@@ -5047,7 +5063,7 @@
       <c r="V8" s="35"/>
     </row>
     <row r="9" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C9" s="107" t="s">
+      <c r="C9" s="121" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="25">
@@ -5059,29 +5075,29 @@
       <c r="F9" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="120" t="s">
+      <c r="H9" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="121"/>
-      <c r="J9" s="122"/>
-      <c r="L9" s="96" t="s">
+      <c r="I9" s="102"/>
+      <c r="J9" s="103"/>
+      <c r="L9" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="97"/>
-      <c r="N9" s="98"/>
-      <c r="P9" s="96" t="s">
+      <c r="M9" s="94"/>
+      <c r="N9" s="95"/>
+      <c r="P9" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="Q9" s="97"/>
-      <c r="R9" s="98"/>
-      <c r="T9" s="105"/>
+      <c r="Q9" s="94"/>
+      <c r="R9" s="95"/>
+      <c r="T9" s="119"/>
       <c r="U9" s="27">
         <v>15</v>
       </c>
       <c r="V9" s="33"/>
     </row>
     <row r="10" spans="3:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="107"/>
+      <c r="C10" s="121"/>
       <c r="D10" s="28">
         <v>9</v>
       </c>
@@ -5091,18 +5107,18 @@
       <c r="F10" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="123" t="s">
+      <c r="H10" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="124"/>
-      <c r="J10" s="125"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="106"/>
       <c r="L10" s="76"/>
-      <c r="M10" s="97"/>
-      <c r="N10" s="98"/>
+      <c r="M10" s="94"/>
+      <c r="N10" s="95"/>
       <c r="P10" s="76"/>
-      <c r="Q10" s="97"/>
-      <c r="R10" s="98"/>
-      <c r="T10" s="104" t="s">
+      <c r="Q10" s="94"/>
+      <c r="R10" s="95"/>
+      <c r="T10" s="118" t="s">
         <v>4</v>
       </c>
       <c r="U10" s="26">
@@ -5111,7 +5127,7 @@
       <c r="V10" s="29"/>
     </row>
     <row r="11" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="106" t="s">
+      <c r="C11" s="120" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="22">
@@ -5123,15 +5139,15 @@
       <c r="F11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="96"/>
-      <c r="I11" s="126"/>
-      <c r="J11" s="127"/>
+      <c r="H11" s="93"/>
+      <c r="I11" s="107"/>
+      <c r="J11" s="108"/>
       <c r="L11" s="76"/>
-      <c r="M11" s="97"/>
-      <c r="N11" s="98"/>
+      <c r="M11" s="94"/>
+      <c r="N11" s="95"/>
       <c r="P11" s="76"/>
-      <c r="Q11" s="97"/>
-      <c r="R11" s="98"/>
+      <c r="Q11" s="94"/>
+      <c r="R11" s="95"/>
       <c r="T11" s="72"/>
       <c r="U11" s="36">
         <v>7</v>
@@ -5139,7 +5155,7 @@
       <c r="V11" s="37"/>
     </row>
     <row r="12" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C12" s="107"/>
+      <c r="C12" s="121"/>
       <c r="D12" s="22">
         <v>12</v>
       </c>
@@ -5149,18 +5165,18 @@
       <c r="F12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="96"/>
-      <c r="I12" s="126"/>
-      <c r="J12" s="127"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="108"/>
       <c r="L12" s="76"/>
-      <c r="M12" s="97"/>
-      <c r="N12" s="98"/>
+      <c r="M12" s="94"/>
+      <c r="N12" s="95"/>
       <c r="P12" s="76"/>
-      <c r="Q12" s="97"/>
-      <c r="R12" s="98"/>
+      <c r="Q12" s="94"/>
+      <c r="R12" s="95"/>
     </row>
     <row r="13" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="108"/>
+      <c r="C13" s="122"/>
       <c r="D13" s="24">
         <v>13</v>
       </c>
@@ -5170,162 +5186,151 @@
       <c r="F13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="96"/>
-      <c r="I13" s="126"/>
-      <c r="J13" s="127"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="107"/>
+      <c r="J13" s="108"/>
       <c r="L13" s="76"/>
-      <c r="M13" s="97"/>
-      <c r="N13" s="98"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="95"/>
       <c r="P13" s="76"/>
-      <c r="Q13" s="97"/>
-      <c r="R13" s="98"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="95"/>
     </row>
     <row r="14" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C14" s="93" t="s">
+      <c r="C14" s="112" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="95"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="126"/>
-      <c r="J14" s="127"/>
+      <c r="D14" s="113"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="114"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="108"/>
       <c r="L14" s="76"/>
-      <c r="M14" s="97"/>
-      <c r="N14" s="98"/>
+      <c r="M14" s="94"/>
+      <c r="N14" s="95"/>
       <c r="P14" s="76"/>
-      <c r="Q14" s="97"/>
-      <c r="R14" s="98"/>
+      <c r="Q14" s="94"/>
+      <c r="R14" s="95"/>
     </row>
     <row r="15" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C15" s="96" t="s">
+      <c r="C15" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98"/>
-      <c r="H15" s="96"/>
-      <c r="I15" s="126"/>
-      <c r="J15" s="127"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="95"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="107"/>
+      <c r="J15" s="108"/>
       <c r="L15" s="76"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="98"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="95"/>
       <c r="P15" s="76"/>
-      <c r="Q15" s="97"/>
-      <c r="R15" s="98"/>
+      <c r="Q15" s="94"/>
+      <c r="R15" s="95"/>
     </row>
     <row r="16" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="72"/>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="100"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="126"/>
-      <c r="J16" s="127"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="97"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="107"/>
+      <c r="J16" s="108"/>
       <c r="L16" s="72"/>
-      <c r="M16" s="99"/>
-      <c r="N16" s="100"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="97"/>
       <c r="P16" s="72"/>
-      <c r="Q16" s="99"/>
-      <c r="R16" s="100"/>
+      <c r="Q16" s="96"/>
+      <c r="R16" s="97"/>
     </row>
     <row r="17" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H17" s="96"/>
-      <c r="I17" s="126"/>
-      <c r="J17" s="127"/>
-      <c r="L17" s="93" t="s">
+      <c r="H17" s="93"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="108"/>
+      <c r="L17" s="112" t="s">
         <v>45</v>
       </c>
-      <c r="M17" s="94"/>
-      <c r="N17" s="95"/>
-      <c r="P17" s="93" t="s">
+      <c r="M17" s="113"/>
+      <c r="N17" s="114"/>
+      <c r="P17" s="112" t="s">
         <v>45</v>
       </c>
-      <c r="Q17" s="94"/>
-      <c r="R17" s="95"/>
+      <c r="Q17" s="113"/>
+      <c r="R17" s="114"/>
     </row>
     <row r="18" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H18" s="96"/>
-      <c r="I18" s="126"/>
-      <c r="J18" s="127"/>
-      <c r="L18" s="96" t="s">
+      <c r="H18" s="93"/>
+      <c r="I18" s="107"/>
+      <c r="J18" s="108"/>
+      <c r="L18" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="M18" s="97"/>
-      <c r="N18" s="98"/>
-      <c r="P18" s="96" t="s">
+      <c r="M18" s="94"/>
+      <c r="N18" s="95"/>
+      <c r="P18" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="Q18" s="97"/>
-      <c r="R18" s="98"/>
+      <c r="Q18" s="94"/>
+      <c r="R18" s="95"/>
     </row>
     <row r="19" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H19" s="128"/>
-      <c r="I19" s="129"/>
-      <c r="J19" s="130"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="110"/>
+      <c r="J19" s="111"/>
       <c r="L19" s="76"/>
-      <c r="M19" s="97"/>
-      <c r="N19" s="98"/>
+      <c r="M19" s="94"/>
+      <c r="N19" s="95"/>
       <c r="P19" s="72"/>
-      <c r="Q19" s="99"/>
-      <c r="R19" s="100"/>
+      <c r="Q19" s="96"/>
+      <c r="R19" s="97"/>
     </row>
     <row r="20" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H20" s="93" t="s">
+      <c r="H20" s="112" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="94"/>
-      <c r="J20" s="95"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="114"/>
       <c r="L20" s="76"/>
-      <c r="M20" s="97"/>
-      <c r="N20" s="98"/>
+      <c r="M20" s="94"/>
+      <c r="N20" s="95"/>
     </row>
     <row r="21" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H21" s="96" t="s">
+      <c r="H21" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="97"/>
-      <c r="J21" s="98"/>
+      <c r="I21" s="94"/>
+      <c r="J21" s="95"/>
       <c r="L21" s="76"/>
-      <c r="M21" s="97"/>
-      <c r="N21" s="98"/>
+      <c r="M21" s="94"/>
+      <c r="N21" s="95"/>
     </row>
     <row r="22" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H22" s="76"/>
-      <c r="I22" s="97"/>
-      <c r="J22" s="98"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="95"/>
       <c r="L22" s="72"/>
-      <c r="M22" s="99"/>
-      <c r="N22" s="100"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="97"/>
     </row>
     <row r="23" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H23" s="76"/>
-      <c r="I23" s="97"/>
-      <c r="J23" s="98"/>
+      <c r="I23" s="94"/>
+      <c r="J23" s="95"/>
     </row>
     <row r="24" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H24" s="76"/>
-      <c r="I24" s="97"/>
-      <c r="J24" s="98"/>
+      <c r="I24" s="94"/>
+      <c r="J24" s="95"/>
     </row>
     <row r="25" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H25" s="72"/>
-      <c r="I25" s="99"/>
-      <c r="J25" s="100"/>
+      <c r="I25" s="96"/>
+      <c r="J25" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="L9:N16"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R16"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J19"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L18:N22"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J25"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C15:F16"/>
     <mergeCell ref="T4:V4"/>
@@ -5342,6 +5347,17 @@
     <mergeCell ref="P6:P7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N16"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R16"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J19"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="L18:N22"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
shield 7 ADCs e perifericos
</commit_message>
<xml_diff>
--- a/04Code/Perifericos.xlsx
+++ b/04Code/Perifericos.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\3ano\2semestre\LPI II\DWR-19\04Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68DE7DB-B48A-4843-A519-F34CDCF354C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE86BCD-29EA-4EFB-8B8F-F17C402BE814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinos Usados" sheetId="1" r:id="rId1"/>
     <sheet name="STM32" sheetId="3" r:id="rId2"/>
-    <sheet name="Perifericos e configurações" sheetId="2" r:id="rId3"/>
+    <sheet name="STM_ADC" sheetId="4" r:id="rId3"/>
+    <sheet name="Perifericos e configurações" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="294">
   <si>
     <t>Porto</t>
   </si>
@@ -924,6 +925,21 @@
   </si>
   <si>
     <t>PWM Left</t>
+  </si>
+  <si>
+    <t>RFID (SDA)</t>
+  </si>
+  <si>
+    <t>RFID (RSET)</t>
+  </si>
+  <si>
+    <t>PE_9</t>
+  </si>
+  <si>
+    <t>ADC3/13</t>
+  </si>
+  <si>
+    <t>ADC2/3</t>
   </si>
 </sst>
 </file>
@@ -1814,195 +1830,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2011,6 +1838,195 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2295,7 +2311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:AW88"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
@@ -2357,14 +2373,14 @@
       </c>
     </row>
     <row r="10" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="74" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
       </c>
       <c r="E10" s="47"/>
-      <c r="G10" s="68" t="s">
+      <c r="G10" s="74" t="s">
         <v>6</v>
       </c>
       <c r="H10" s="3">
@@ -2373,7 +2389,7 @@
       <c r="I10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="76" t="s">
+      <c r="K10" s="82" t="s">
         <v>8</v>
       </c>
       <c r="L10" s="3">
@@ -2382,290 +2398,290 @@
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="69"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="5">
         <v>1</v>
       </c>
       <c r="E11" s="21"/>
-      <c r="G11" s="69"/>
+      <c r="G11" s="75"/>
       <c r="H11" s="7">
         <v>1</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="76"/>
+      <c r="K11" s="82"/>
       <c r="L11" s="7">
         <v>1</v>
       </c>
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="69"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="5">
         <v>2</v>
       </c>
       <c r="E12" s="21"/>
-      <c r="G12" s="69"/>
+      <c r="G12" s="75"/>
       <c r="H12" s="7">
         <v>2</v>
       </c>
       <c r="I12" s="6"/>
-      <c r="K12" s="76"/>
+      <c r="K12" s="82"/>
       <c r="L12" s="7">
         <v>2</v>
       </c>
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="69"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="7">
         <v>3</v>
       </c>
       <c r="E13" s="21"/>
-      <c r="G13" s="69"/>
+      <c r="G13" s="75"/>
       <c r="H13" s="7">
         <v>3</v>
       </c>
       <c r="I13" s="6"/>
-      <c r="K13" s="76"/>
+      <c r="K13" s="82"/>
       <c r="L13" s="7">
         <v>3</v>
       </c>
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="69"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="7">
         <v>4</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="69"/>
+      <c r="G14" s="75"/>
       <c r="H14" s="7">
         <v>4</v>
       </c>
       <c r="I14" s="6"/>
-      <c r="K14" s="76"/>
+      <c r="K14" s="82"/>
       <c r="L14" s="5">
         <v>4</v>
       </c>
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="69"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="7">
         <v>5</v>
       </c>
       <c r="E15" s="21"/>
-      <c r="G15" s="69"/>
+      <c r="G15" s="75"/>
       <c r="H15" s="7">
         <v>5</v>
       </c>
       <c r="I15" s="6"/>
-      <c r="K15" s="76"/>
+      <c r="K15" s="82"/>
       <c r="L15" s="5">
         <v>5</v>
       </c>
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="69"/>
+      <c r="C16" s="75"/>
       <c r="D16" s="7">
         <v>6</v>
       </c>
       <c r="E16" s="50" t="s">
         <v>285</v>
       </c>
-      <c r="G16" s="69"/>
+      <c r="G16" s="75"/>
       <c r="H16" s="7">
         <v>6</v>
       </c>
       <c r="I16" s="6"/>
-      <c r="K16" s="76"/>
+      <c r="K16" s="82"/>
       <c r="L16" s="5">
         <v>6</v>
       </c>
       <c r="M16" s="6"/>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="69"/>
+      <c r="C17" s="75"/>
       <c r="D17" s="7">
         <v>7</v>
       </c>
       <c r="E17" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="G17" s="69"/>
+      <c r="G17" s="75"/>
       <c r="H17" s="7">
         <v>7</v>
       </c>
       <c r="I17" s="6"/>
-      <c r="K17" s="76"/>
+      <c r="K17" s="82"/>
       <c r="L17" s="5">
         <v>7</v>
       </c>
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="69"/>
+      <c r="C18" s="75"/>
       <c r="D18" s="5">
         <v>8</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="G18" s="69"/>
+      <c r="G18" s="75"/>
       <c r="H18" s="5">
         <v>8</v>
       </c>
       <c r="I18" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="76"/>
+      <c r="K18" s="82"/>
       <c r="L18" s="5">
         <v>8</v>
       </c>
       <c r="M18" s="6"/>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C19" s="69"/>
+      <c r="C19" s="75"/>
       <c r="D19" s="5">
         <v>9</v>
       </c>
       <c r="E19" s="6"/>
-      <c r="G19" s="69"/>
+      <c r="G19" s="75"/>
       <c r="H19" s="5">
         <v>9</v>
       </c>
       <c r="I19" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K19" s="76"/>
+      <c r="K19" s="82"/>
       <c r="L19" s="7">
         <v>9</v>
       </c>
       <c r="M19" s="6"/>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C20" s="69"/>
+      <c r="C20" s="75"/>
       <c r="D20" s="5">
         <v>10</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="G20" s="69"/>
+      <c r="G20" s="75"/>
       <c r="H20" s="5">
         <v>10</v>
       </c>
       <c r="I20" s="6"/>
-      <c r="K20" s="76"/>
+      <c r="K20" s="82"/>
       <c r="L20" s="5">
         <v>10</v>
       </c>
       <c r="M20" s="6"/>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C21" s="69"/>
+      <c r="C21" s="75"/>
       <c r="D21" s="5">
         <v>11</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="G21" s="69"/>
+      <c r="G21" s="75"/>
       <c r="H21" s="7">
         <v>11</v>
       </c>
       <c r="I21" s="6"/>
-      <c r="K21" s="76"/>
+      <c r="K21" s="82"/>
       <c r="L21" s="5">
         <v>11</v>
       </c>
       <c r="M21" s="6"/>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="69"/>
+      <c r="C22" s="75"/>
       <c r="D22" s="5">
         <v>12</v>
       </c>
       <c r="E22" s="6"/>
-      <c r="G22" s="69"/>
+      <c r="G22" s="75"/>
       <c r="H22" s="7">
         <v>12</v>
       </c>
       <c r="I22" s="6"/>
-      <c r="K22" s="76"/>
+      <c r="K22" s="82"/>
       <c r="L22" s="5">
         <v>12</v>
       </c>
       <c r="M22" s="6"/>
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C23" s="69"/>
+      <c r="C23" s="75"/>
       <c r="D23" s="5">
         <v>13</v>
       </c>
       <c r="E23" s="21"/>
-      <c r="G23" s="69"/>
+      <c r="G23" s="75"/>
       <c r="H23" s="7">
         <v>13</v>
       </c>
       <c r="I23" s="6"/>
-      <c r="K23" s="76"/>
+      <c r="K23" s="82"/>
       <c r="L23" s="5">
         <v>13</v>
       </c>
       <c r="M23" s="6"/>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="69"/>
+      <c r="C24" s="75"/>
       <c r="D24" s="5">
         <v>14</v>
       </c>
       <c r="E24" s="21"/>
-      <c r="G24" s="69"/>
+      <c r="G24" s="75"/>
       <c r="H24" s="7">
         <v>14</v>
       </c>
       <c r="I24" s="6"/>
-      <c r="K24" s="76"/>
+      <c r="K24" s="82"/>
       <c r="L24" s="7">
         <v>14</v>
       </c>
       <c r="M24" s="6"/>
     </row>
     <row r="25" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="70"/>
+      <c r="C25" s="76"/>
       <c r="D25" s="8">
         <v>15</v>
       </c>
       <c r="E25" s="48"/>
-      <c r="G25" s="70"/>
+      <c r="G25" s="76"/>
       <c r="H25" s="8">
         <v>15</v>
       </c>
       <c r="I25" s="40" t="s">
         <v>283</v>
       </c>
-      <c r="K25" s="72"/>
+      <c r="K25" s="78"/>
       <c r="L25" s="10">
         <v>15</v>
       </c>
       <c r="M25" s="9"/>
     </row>
     <row r="26" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C26" s="73" t="s">
+      <c r="C26" s="79" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="3">
         <v>0</v>
       </c>
       <c r="E26" s="47"/>
-      <c r="G26" s="73" t="s">
+      <c r="G26" s="79" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="K26" s="71" t="s">
+      <c r="K26" s="77" t="s">
         <v>9</v>
       </c>
       <c r="L26" s="11">
@@ -2674,231 +2690,231 @@
       <c r="M26" s="4"/>
     </row>
     <row r="27" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="74"/>
+      <c r="C27" s="80"/>
       <c r="D27" s="7">
         <v>1</v>
       </c>
       <c r="E27" s="21"/>
-      <c r="G27" s="74"/>
+      <c r="G27" s="80"/>
       <c r="H27" s="5">
         <v>1</v>
       </c>
       <c r="I27" s="6"/>
-      <c r="K27" s="72"/>
+      <c r="K27" s="78"/>
       <c r="L27" s="12">
         <v>1</v>
       </c>
       <c r="M27" s="13"/>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C28" s="74"/>
+      <c r="C28" s="80"/>
       <c r="D28" s="7">
         <v>2</v>
       </c>
       <c r="E28" s="6"/>
-      <c r="G28" s="74"/>
+      <c r="G28" s="80"/>
       <c r="H28" s="7">
         <v>2</v>
       </c>
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C29" s="74"/>
+      <c r="C29" s="80"/>
       <c r="D29" s="5">
         <v>3</v>
       </c>
       <c r="E29" s="6"/>
-      <c r="G29" s="74"/>
+      <c r="G29" s="80"/>
       <c r="H29" s="7">
         <v>3</v>
       </c>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="74"/>
+      <c r="C30" s="80"/>
       <c r="D30" s="7">
         <v>4</v>
       </c>
       <c r="E30" s="6"/>
-      <c r="G30" s="74"/>
+      <c r="G30" s="80"/>
       <c r="H30" s="7">
         <v>4</v>
       </c>
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C31" s="74"/>
+      <c r="C31" s="80"/>
       <c r="D31" s="7">
         <v>5</v>
       </c>
       <c r="E31" s="6"/>
-      <c r="G31" s="74"/>
+      <c r="G31" s="80"/>
       <c r="H31" s="7">
         <v>5</v>
       </c>
       <c r="I31" s="6"/>
-      <c r="K31" s="77" t="s">
+      <c r="K31" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="L31" s="78"/>
-      <c r="M31" s="79"/>
+      <c r="L31" s="84"/>
+      <c r="M31" s="85"/>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C32" s="74"/>
+      <c r="C32" s="80"/>
       <c r="D32" s="7">
         <v>6</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="74"/>
+      <c r="G32" s="80"/>
       <c r="H32" s="7">
         <v>6</v>
       </c>
       <c r="I32" s="6"/>
-      <c r="K32" s="80"/>
-      <c r="L32" s="81"/>
-      <c r="M32" s="82"/>
+      <c r="K32" s="86"/>
+      <c r="L32" s="87"/>
+      <c r="M32" s="88"/>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C33" s="74"/>
+      <c r="C33" s="80"/>
       <c r="D33" s="5">
         <v>7</v>
       </c>
       <c r="E33" s="6"/>
-      <c r="G33" s="74"/>
+      <c r="G33" s="80"/>
       <c r="H33" s="7">
         <v>7</v>
       </c>
       <c r="I33" s="6"/>
-      <c r="K33" s="83"/>
-      <c r="L33" s="81"/>
-      <c r="M33" s="82"/>
+      <c r="K33" s="89"/>
+      <c r="L33" s="87"/>
+      <c r="M33" s="88"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C34" s="74"/>
+      <c r="C34" s="80"/>
       <c r="D34" s="7">
         <v>8</v>
       </c>
       <c r="E34" s="40" t="s">
         <v>274</v>
       </c>
-      <c r="G34" s="74"/>
+      <c r="G34" s="80"/>
       <c r="H34" s="7">
         <v>8</v>
       </c>
       <c r="I34" s="6"/>
-      <c r="K34" s="83"/>
-      <c r="L34" s="81"/>
-      <c r="M34" s="82"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="87"/>
+      <c r="M34" s="88"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C35" s="74"/>
+      <c r="C35" s="80"/>
       <c r="D35" s="7">
         <v>9</v>
       </c>
       <c r="E35" s="40" t="s">
         <v>282</v>
       </c>
-      <c r="G35" s="74"/>
+      <c r="G35" s="80"/>
       <c r="H35" s="7">
         <v>9</v>
       </c>
       <c r="I35" s="6"/>
-      <c r="K35" s="83"/>
-      <c r="L35" s="81"/>
-      <c r="M35" s="82"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="87"/>
+      <c r="M35" s="88"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C36" s="74"/>
+      <c r="C36" s="80"/>
       <c r="D36" s="7">
         <v>10</v>
       </c>
       <c r="E36" s="6"/>
-      <c r="G36" s="74"/>
+      <c r="G36" s="80"/>
       <c r="H36" s="7">
         <v>10</v>
       </c>
       <c r="I36" s="6"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="81"/>
-      <c r="M36" s="82"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="87"/>
+      <c r="M36" s="88"/>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C37" s="74"/>
+      <c r="C37" s="80"/>
       <c r="D37" s="7">
         <v>11</v>
       </c>
       <c r="E37" s="6"/>
-      <c r="G37" s="74"/>
+      <c r="G37" s="80"/>
       <c r="H37" s="7">
         <v>11</v>
       </c>
       <c r="I37" s="6"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="81"/>
-      <c r="M37" s="82"/>
+      <c r="K37" s="89"/>
+      <c r="L37" s="87"/>
+      <c r="M37" s="88"/>
     </row>
     <row r="38" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C38" s="74"/>
+      <c r="C38" s="80"/>
       <c r="D38" s="7">
         <v>12</v>
       </c>
       <c r="E38" s="21"/>
-      <c r="G38" s="74"/>
+      <c r="G38" s="80"/>
       <c r="H38" s="7">
         <v>12</v>
       </c>
       <c r="I38" s="6"/>
-      <c r="K38" s="83"/>
-      <c r="L38" s="81"/>
-      <c r="M38" s="82"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="87"/>
+      <c r="M38" s="88"/>
     </row>
     <row r="39" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="74"/>
+      <c r="C39" s="80"/>
       <c r="D39" s="7">
         <v>13</v>
       </c>
       <c r="E39" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="G39" s="74"/>
+      <c r="G39" s="80"/>
       <c r="H39" s="7">
         <v>13</v>
       </c>
       <c r="I39" s="6"/>
-      <c r="K39" s="84"/>
-      <c r="L39" s="85"/>
-      <c r="M39" s="86"/>
+      <c r="K39" s="90"/>
+      <c r="L39" s="91"/>
+      <c r="M39" s="92"/>
     </row>
     <row r="40" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C40" s="74"/>
+      <c r="C40" s="80"/>
       <c r="D40" s="5">
         <v>14</v>
       </c>
       <c r="E40" s="6"/>
-      <c r="G40" s="74"/>
+      <c r="G40" s="80"/>
       <c r="H40" s="7">
         <v>14</v>
       </c>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="75"/>
+      <c r="C41" s="81"/>
       <c r="D41" s="8">
         <v>15</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="G41" s="75"/>
+      <c r="G41" s="81"/>
       <c r="H41" s="8">
         <v>15</v>
       </c>
       <c r="I41" s="9"/>
     </row>
     <row r="42" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="68" t="s">
+      <c r="C42" s="74" t="s">
         <v>4</v>
       </c>
       <c r="D42" s="3">
@@ -2907,7 +2923,7 @@
       <c r="E42" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G42" s="68" t="s">
+      <c r="G42" s="74" t="s">
         <v>7</v>
       </c>
       <c r="H42" s="3">
@@ -2918,12 +2934,12 @@
       </c>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C43" s="69"/>
+      <c r="C43" s="75"/>
       <c r="D43" s="5">
         <v>1</v>
       </c>
       <c r="E43" s="6"/>
-      <c r="G43" s="69"/>
+      <c r="G43" s="75"/>
       <c r="H43" s="7">
         <v>1</v>
       </c>
@@ -2932,138 +2948,138 @@
       </c>
     </row>
     <row r="44" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C44" s="69"/>
+      <c r="C44" s="75"/>
       <c r="D44" s="7">
         <v>2</v>
       </c>
       <c r="E44" s="21"/>
-      <c r="G44" s="69"/>
+      <c r="G44" s="75"/>
       <c r="H44" s="7">
         <v>2</v>
       </c>
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="69"/>
+      <c r="C45" s="75"/>
       <c r="D45" s="7">
         <v>3</v>
       </c>
       <c r="E45" s="21"/>
-      <c r="G45" s="69"/>
+      <c r="G45" s="75"/>
       <c r="H45" s="7">
         <v>3</v>
       </c>
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="69"/>
+      <c r="C46" s="75"/>
       <c r="D46" s="5">
         <v>4</v>
       </c>
       <c r="E46" s="21"/>
-      <c r="G46" s="69"/>
+      <c r="G46" s="75"/>
       <c r="H46" s="7">
         <v>4</v>
       </c>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="69"/>
+      <c r="C47" s="75"/>
       <c r="D47" s="5">
         <v>5</v>
       </c>
       <c r="E47" s="21"/>
-      <c r="G47" s="69"/>
+      <c r="G47" s="75"/>
       <c r="H47" s="7">
         <v>5</v>
       </c>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="69"/>
+      <c r="C48" s="75"/>
       <c r="D48" s="7">
         <v>6</v>
       </c>
       <c r="E48" s="21"/>
-      <c r="G48" s="69"/>
+      <c r="G48" s="75"/>
       <c r="H48" s="5">
         <v>6</v>
       </c>
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="69"/>
+      <c r="C49" s="75"/>
       <c r="D49" s="7">
         <v>7</v>
       </c>
       <c r="E49" s="21"/>
-      <c r="G49" s="69"/>
+      <c r="G49" s="75"/>
       <c r="H49" s="7">
         <v>7</v>
       </c>
       <c r="I49" s="6"/>
     </row>
     <row r="50" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="69"/>
+      <c r="C50" s="75"/>
       <c r="D50" s="7">
         <v>8</v>
       </c>
       <c r="E50" s="21"/>
-      <c r="G50" s="69"/>
+      <c r="G50" s="75"/>
       <c r="H50" s="7">
         <v>8</v>
       </c>
       <c r="I50" s="6"/>
     </row>
     <row r="51" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="69"/>
+      <c r="C51" s="75"/>
       <c r="D51" s="7">
         <v>9</v>
       </c>
       <c r="E51" s="6"/>
-      <c r="G51" s="69"/>
+      <c r="G51" s="75"/>
       <c r="H51" s="7">
         <v>9</v>
       </c>
       <c r="I51" s="6"/>
     </row>
     <row r="52" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="69"/>
+      <c r="C52" s="75"/>
       <c r="D52" s="7">
         <v>10</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G52" s="69"/>
+      <c r="G52" s="75"/>
       <c r="H52" s="7">
         <v>10</v>
       </c>
       <c r="I52" s="6"/>
     </row>
     <row r="53" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="69"/>
+      <c r="C53" s="75"/>
       <c r="D53" s="7">
         <v>11</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G53" s="69"/>
+      <c r="G53" s="75"/>
       <c r="H53" s="5">
         <v>11</v>
       </c>
       <c r="I53" s="6"/>
     </row>
     <row r="54" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="69"/>
+      <c r="C54" s="75"/>
       <c r="D54" s="7">
         <v>12</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G54" s="69"/>
+      <c r="G54" s="75"/>
       <c r="H54" s="7">
         <v>12</v>
       </c>
@@ -3072,12 +3088,12 @@
       </c>
     </row>
     <row r="55" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C55" s="69"/>
+      <c r="C55" s="75"/>
       <c r="D55" s="5">
         <v>13</v>
       </c>
       <c r="E55" s="6"/>
-      <c r="G55" s="69"/>
+      <c r="G55" s="75"/>
       <c r="H55" s="7">
         <v>13</v>
       </c>
@@ -3086,24 +3102,24 @@
       </c>
     </row>
     <row r="56" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="69"/>
+      <c r="C56" s="75"/>
       <c r="D56" s="5">
         <v>14</v>
       </c>
       <c r="E56" s="6"/>
-      <c r="G56" s="69"/>
+      <c r="G56" s="75"/>
       <c r="H56" s="7">
         <v>14</v>
       </c>
       <c r="I56" s="6"/>
     </row>
     <row r="57" spans="3:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="70"/>
+      <c r="C57" s="76"/>
       <c r="D57" s="10">
         <v>15</v>
       </c>
       <c r="E57" s="9"/>
-      <c r="G57" s="70"/>
+      <c r="G57" s="76"/>
       <c r="H57" s="8">
         <v>15</v>
       </c>
@@ -3162,8 +3178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D1835F-16BF-4BB4-AE8E-49185A3BFF21}">
   <dimension ref="A4:AH33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView topLeftCell="B13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,42 +3191,42 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="93" t="s">
         <v>278</v>
       </c>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="91" t="s">
+      <c r="R4" s="97" t="s">
         <v>280</v>
       </c>
-      <c r="S4" s="92"/>
-      <c r="T4" s="92"/>
-      <c r="U4" s="92"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="92"/>
-      <c r="X4" s="92"/>
-      <c r="Y4" s="92"/>
-      <c r="Z4" s="92"/>
-      <c r="AA4" s="92"/>
-      <c r="AB4" s="92"/>
-      <c r="AC4" s="92"/>
-      <c r="AD4" s="92"/>
-      <c r="AE4" s="92"/>
-      <c r="AF4" s="92"/>
-      <c r="AG4" s="92"/>
-      <c r="AH4" s="92"/>
+      <c r="S4" s="98"/>
+      <c r="T4" s="98"/>
+      <c r="U4" s="98"/>
+      <c r="V4" s="98"/>
+      <c r="W4" s="98"/>
+      <c r="X4" s="98"/>
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="98"/>
+      <c r="AA4" s="98"/>
+      <c r="AB4" s="98"/>
+      <c r="AC4" s="98"/>
+      <c r="AD4" s="98"/>
+      <c r="AE4" s="98"/>
+      <c r="AF4" s="98"/>
+      <c r="AG4" s="98"/>
+      <c r="AH4" s="98"/>
     </row>
     <row r="5" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="61"/>
@@ -3233,7 +3249,9 @@
       <c r="L5" s="52"/>
       <c r="M5" s="52"/>
       <c r="N5" s="56"/>
-      <c r="O5" s="57"/>
+      <c r="O5" s="57" t="s">
+        <v>290</v>
+      </c>
       <c r="P5" s="42"/>
       <c r="Q5" s="42"/>
       <c r="R5" s="57" t="s">
@@ -3559,7 +3577,9 @@
       <c r="L10" s="52"/>
       <c r="M10" s="52"/>
       <c r="N10" s="56"/>
-      <c r="O10" s="57"/>
+      <c r="O10" s="57" t="s">
+        <v>289</v>
+      </c>
       <c r="P10" s="42"/>
       <c r="Q10" s="42"/>
       <c r="R10" s="57"/>
@@ -3580,7 +3600,7 @@
       <c r="AA10" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="AB10" s="135" t="s">
+      <c r="AB10" s="72" t="s">
         <v>176</v>
       </c>
       <c r="AC10" s="52" t="s">
@@ -3640,7 +3660,7 @@
       <c r="AA11" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="AB11" s="135" t="s">
+      <c r="AB11" s="72" t="s">
         <v>198</v>
       </c>
       <c r="AC11" s="52" t="s">
@@ -3763,8 +3783,8 @@
       </c>
     </row>
     <row r="14" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="131"/>
-      <c r="B14" s="131"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="57" t="s">
         <v>276</v>
       </c>
@@ -3829,7 +3849,7 @@
       <c r="AH14" s="60"/>
     </row>
     <row r="15" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="131"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="44"/>
       <c r="C15" s="57" t="s">
         <v>25</v>
@@ -3837,7 +3857,7 @@
       <c r="D15" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="E15" s="136" t="s">
+      <c r="E15" s="73" t="s">
         <v>135</v>
       </c>
       <c r="F15" s="52"/>
@@ -3879,8 +3899,8 @@
       <c r="AH15" s="44"/>
     </row>
     <row r="16" spans="1:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="131"/>
-      <c r="B16" s="131"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="57" t="s">
         <v>27</v>
       </c>
@@ -3970,7 +3990,7 @@
         <v>227</v>
       </c>
       <c r="AA17" s="54" t="s">
-        <v>90</v>
+        <v>291</v>
       </c>
       <c r="AB17" s="56" t="s">
         <v>239</v>
@@ -4039,7 +4059,7 @@
       <c r="AH18" s="57"/>
     </row>
     <row r="19" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="133"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="56" t="s">
         <v>146</v>
       </c>
@@ -4093,7 +4113,7 @@
       <c r="AH19" s="57"/>
     </row>
     <row r="20" spans="3:34" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="132"/>
+      <c r="C20" s="69"/>
       <c r="D20" s="56"/>
       <c r="E20" s="52"/>
       <c r="F20" s="52"/>
@@ -4269,7 +4289,7 @@
       <c r="AH22" s="57"/>
     </row>
     <row r="23" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="133"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="56"/>
       <c r="E23" s="56" t="s">
         <v>149</v>
@@ -4325,7 +4345,7 @@
       <c r="AH23" s="57"/>
     </row>
     <row r="24" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="134"/>
+      <c r="C24" s="71"/>
       <c r="D24" s="56"/>
       <c r="E24" s="56" t="s">
         <v>150</v>
@@ -4433,7 +4453,7 @@
       <c r="AH25" s="57"/>
     </row>
     <row r="26" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="134"/>
+      <c r="C26" s="71"/>
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
       <c r="F26" s="56" t="s">
@@ -4495,7 +4515,7 @@
       <c r="AH26" s="57"/>
     </row>
     <row r="27" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="132"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="56"/>
       <c r="E27" s="56"/>
       <c r="F27" s="56" t="s">
@@ -4609,21 +4629,21 @@
       <c r="AH28" s="57"/>
     </row>
     <row r="29" spans="3:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="89" t="s">
+      <c r="C29" s="95" t="s">
         <v>279</v>
       </c>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="90"/>
-      <c r="N29" s="90"/>
-      <c r="O29" s="90"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="96"/>
+      <c r="F29" s="96"/>
+      <c r="G29" s="96"/>
+      <c r="H29" s="96"/>
+      <c r="I29" s="96"/>
+      <c r="J29" s="96"/>
+      <c r="K29" s="96"/>
+      <c r="L29" s="96"/>
+      <c r="M29" s="96"/>
+      <c r="N29" s="96"/>
+      <c r="O29" s="96"/>
       <c r="P29" s="43"/>
       <c r="Q29" s="42"/>
       <c r="R29" s="61"/>
@@ -4816,25 +4836,25 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="89" t="s">
+      <c r="R33" s="95" t="s">
         <v>281</v>
       </c>
-      <c r="S33" s="90"/>
-      <c r="T33" s="90"/>
-      <c r="U33" s="90"/>
-      <c r="V33" s="90"/>
-      <c r="W33" s="90"/>
-      <c r="X33" s="90"/>
-      <c r="Y33" s="90"/>
-      <c r="Z33" s="90"/>
-      <c r="AA33" s="90"/>
-      <c r="AB33" s="90"/>
-      <c r="AC33" s="90"/>
-      <c r="AD33" s="90"/>
-      <c r="AE33" s="90"/>
-      <c r="AF33" s="90"/>
-      <c r="AG33" s="90"/>
-      <c r="AH33" s="90"/>
+      <c r="S33" s="96"/>
+      <c r="T33" s="96"/>
+      <c r="U33" s="96"/>
+      <c r="V33" s="96"/>
+      <c r="W33" s="96"/>
+      <c r="X33" s="96"/>
+      <c r="Y33" s="96"/>
+      <c r="Z33" s="96"/>
+      <c r="AA33" s="96"/>
+      <c r="AB33" s="96"/>
+      <c r="AC33" s="96"/>
+      <c r="AD33" s="96"/>
+      <c r="AE33" s="96"/>
+      <c r="AF33" s="96"/>
+      <c r="AG33" s="96"/>
+      <c r="AH33" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4849,6 +4869,1697 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FE4C32-C97D-45A9-AB28-ECC31E431526}">
+  <dimension ref="A1:AJ32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21:H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="54"/>
+    </row>
+    <row r="3" spans="1:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="93" t="s">
+        <v>278</v>
+      </c>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="97" t="s">
+        <v>280</v>
+      </c>
+      <c r="U3" s="98"/>
+      <c r="V3" s="98"/>
+      <c r="W3" s="98"/>
+      <c r="X3" s="98"/>
+      <c r="Y3" s="98"/>
+      <c r="Z3" s="98"/>
+      <c r="AA3" s="98"/>
+      <c r="AB3" s="98"/>
+      <c r="AC3" s="98"/>
+      <c r="AD3" s="98"/>
+      <c r="AE3" s="98"/>
+      <c r="AF3" s="98"/>
+      <c r="AG3" s="98"/>
+      <c r="AH3" s="98"/>
+      <c r="AI3" s="98"/>
+      <c r="AJ3" s="98"/>
+    </row>
+    <row r="4" spans="1:36" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="61"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="57" t="s">
+        <v>277</v>
+      </c>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56"/>
+      <c r="Z4" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="AA4" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB4" s="51" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC4" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD4" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE4" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF4" s="56" t="s">
+        <v>163</v>
+      </c>
+      <c r="AG4" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="AH4" s="56"/>
+      <c r="AI4" s="56"/>
+      <c r="AJ4" s="57" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="61"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="57" t="s">
+        <v>268</v>
+      </c>
+      <c r="U5" s="56"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="X5" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y5" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z5" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA5" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB5" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC5" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD5" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE5" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF5" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG5" s="52" t="s">
+        <v>173</v>
+      </c>
+      <c r="AH5" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="AI5" s="52"/>
+      <c r="AJ5" s="61" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="61"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="56" t="s">
+        <v>192</v>
+      </c>
+      <c r="V6" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="W6" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="X6" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y6" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z6" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA6" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB6" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC6" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD6" s="52"/>
+      <c r="AE6" s="52"/>
+      <c r="AF6" s="52"/>
+      <c r="AG6" s="52"/>
+      <c r="AH6" s="52"/>
+      <c r="AI6" s="52"/>
+      <c r="AJ6" s="61"/>
+    </row>
+    <row r="7" spans="1:36" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="61"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="56" t="s">
+        <v>197</v>
+      </c>
+      <c r="V7" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="W7" s="52" t="s">
+        <v>203</v>
+      </c>
+      <c r="X7" s="52" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y7" s="52"/>
+      <c r="Z7" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA7" s="52"/>
+      <c r="AB7" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC7" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD7" s="52"/>
+      <c r="AE7" s="52"/>
+      <c r="AF7" s="52"/>
+      <c r="AG7" s="52"/>
+      <c r="AH7" s="52"/>
+      <c r="AI7" s="52"/>
+      <c r="AJ7" s="61"/>
+    </row>
+    <row r="8" spans="1:36" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="61"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="M8" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="56"/>
+      <c r="V8" s="52"/>
+      <c r="W8" s="52" t="s">
+        <v>195</v>
+      </c>
+      <c r="X8" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y8" s="52" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z8" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA8" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB8" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="AC8" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD8" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE8" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF8" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG8" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="AH8" s="52"/>
+      <c r="AI8" s="52" t="s">
+        <v>259</v>
+      </c>
+      <c r="AJ8" s="61" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="E9" s="61"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="K9" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="46"/>
+      <c r="M9" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="57"/>
+      <c r="U9" s="56"/>
+      <c r="V9" s="52"/>
+      <c r="W9" s="52"/>
+      <c r="X9" s="52"/>
+      <c r="Y9" s="52"/>
+      <c r="Z9" s="52" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA9" s="52" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB9" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC9" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD9" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="AE9" s="52" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF9" s="52"/>
+      <c r="AG9" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="AH9" s="52"/>
+      <c r="AI9" s="52"/>
+      <c r="AJ9" s="61" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="E10" s="61"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="61"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="56"/>
+      <c r="V10" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="W10" s="52" t="s">
+        <v>203</v>
+      </c>
+      <c r="X10" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y10" s="52"/>
+      <c r="Z10" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA10" s="52" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB10" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC10" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD10" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE10" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF10" s="52"/>
+      <c r="AG10" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH10" s="52"/>
+      <c r="AI10" s="52"/>
+      <c r="AJ10" s="61"/>
+    </row>
+    <row r="11" spans="1:36" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="57"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="56"/>
+      <c r="V11" s="52"/>
+      <c r="W11" s="52" t="s">
+        <v>207</v>
+      </c>
+      <c r="X11" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y11" s="52"/>
+      <c r="Z11" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA11" s="52" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB11" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC11" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD11" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE11" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="AF11" s="52"/>
+      <c r="AG11" s="52"/>
+      <c r="AH11" s="52"/>
+      <c r="AI11" s="52"/>
+      <c r="AJ11" s="61" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="56"/>
+      <c r="V12" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="W12" s="52"/>
+      <c r="X12" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y12" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z12" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA12" s="52"/>
+      <c r="AB12" s="51" t="s">
+        <v>170</v>
+      </c>
+      <c r="AC12" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="AD12" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE12" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF12" s="52"/>
+      <c r="AG12" s="52"/>
+      <c r="AH12" s="52"/>
+      <c r="AI12" s="52"/>
+      <c r="AJ12" s="61" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" s="55" t="s">
+        <v>293</v>
+      </c>
+      <c r="H13" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="J13" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="61"/>
+      <c r="U13" s="52"/>
+      <c r="V13" s="52"/>
+      <c r="W13" s="52" t="s">
+        <v>195</v>
+      </c>
+      <c r="X13" s="52" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y13" s="52" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z13" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA13" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB13" s="65" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC13" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD13" s="46"/>
+      <c r="AE13" s="52"/>
+      <c r="AF13" s="52"/>
+      <c r="AG13" s="52"/>
+      <c r="AH13" s="52"/>
+      <c r="AI13" s="52"/>
+      <c r="AJ13" s="60"/>
+    </row>
+    <row r="14" spans="1:36" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="68"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="K14" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="L14" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="M14" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="44"/>
+      <c r="X14" s="44"/>
+      <c r="Y14" s="44"/>
+      <c r="Z14" s="44"/>
+      <c r="AA14" s="44"/>
+      <c r="AB14" s="43"/>
+      <c r="AC14" s="43"/>
+      <c r="AD14" s="44"/>
+      <c r="AE14" s="44"/>
+      <c r="AF14" s="44"/>
+      <c r="AG14" s="44"/>
+      <c r="AH14" s="44"/>
+      <c r="AI14" s="44"/>
+      <c r="AJ14" s="44"/>
+    </row>
+    <row r="15" spans="1:36" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="55" t="s">
+        <v>292</v>
+      </c>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="J15" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="K15" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="53"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="53"/>
+      <c r="Y15" s="53"/>
+      <c r="Z15" s="45"/>
+      <c r="AA15" s="53"/>
+      <c r="AB15" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC15" s="67" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD15" s="53"/>
+      <c r="AE15" s="53"/>
+      <c r="AF15" s="53"/>
+      <c r="AG15" s="53"/>
+      <c r="AH15" s="53"/>
+      <c r="AI15" s="53"/>
+      <c r="AJ15" s="62"/>
+    </row>
+    <row r="16" spans="1:36" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="56"/>
+      <c r="G16" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="K16" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="62"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="53"/>
+      <c r="W16" s="53"/>
+      <c r="X16" s="53"/>
+      <c r="Y16" s="53"/>
+      <c r="Z16" s="56"/>
+      <c r="AA16" s="52"/>
+      <c r="AB16" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC16" s="54" t="s">
+        <v>291</v>
+      </c>
+      <c r="AD16" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE16" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF16" s="56"/>
+      <c r="AG16" s="56"/>
+      <c r="AH16" s="56"/>
+      <c r="AI16" s="56"/>
+      <c r="AJ16" s="57"/>
+    </row>
+    <row r="17" spans="5:36" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="56"/>
+      <c r="G17" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="K17" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="L17" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="M17" s="56" t="s">
+        <v>109</v>
+      </c>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="42"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="57"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
+      <c r="Y17" s="56"/>
+      <c r="Z17" s="56"/>
+      <c r="AA17" s="56"/>
+      <c r="AB17" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC17" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="AD17" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="AE17" s="56"/>
+      <c r="AF17" s="56"/>
+      <c r="AG17" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH17" s="56"/>
+      <c r="AI17" s="56"/>
+      <c r="AJ17" s="57"/>
+    </row>
+    <row r="18" spans="5:36" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="G18" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="K18" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="58"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="58"/>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="42"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="52"/>
+      <c r="V18" s="52" t="s">
+        <v>262</v>
+      </c>
+      <c r="W18" s="52"/>
+      <c r="X18" s="52"/>
+      <c r="Y18" s="52"/>
+      <c r="Z18" s="52" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA18" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB18" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC18" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD18" s="56"/>
+      <c r="AE18" s="56"/>
+      <c r="AF18" s="56" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG18" s="56"/>
+      <c r="AH18" s="56"/>
+      <c r="AI18" s="56"/>
+      <c r="AJ18" s="57"/>
+    </row>
+    <row r="19" spans="5:36" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="69"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="L19" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="57"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="61"/>
+      <c r="U19" s="52"/>
+      <c r="V19" s="52" t="s">
+        <v>265</v>
+      </c>
+      <c r="W19" s="52"/>
+      <c r="X19" s="52" t="s">
+        <v>250</v>
+      </c>
+      <c r="Y19" s="52"/>
+      <c r="Z19" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA19" s="52"/>
+      <c r="AB19" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC19" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD19" s="56" t="s">
+        <v>241</v>
+      </c>
+      <c r="AE19" s="56"/>
+      <c r="AF19" s="56"/>
+      <c r="AG19" s="56" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH19" s="56"/>
+      <c r="AI19" s="56"/>
+      <c r="AJ19" s="57"/>
+    </row>
+    <row r="20" spans="5:36" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="56"/>
+      <c r="G20" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="H20" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="I20" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="J20" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="K20" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="61"/>
+      <c r="U20" s="52"/>
+      <c r="V20" s="52"/>
+      <c r="W20" s="52"/>
+      <c r="X20" s="52"/>
+      <c r="Y20" s="52"/>
+      <c r="Z20" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA20" s="52"/>
+      <c r="AB20" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC20" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD20" s="56"/>
+      <c r="AE20" s="56"/>
+      <c r="AF20" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="AG20" s="56"/>
+      <c r="AH20" s="56"/>
+      <c r="AI20" s="56"/>
+      <c r="AJ20" s="57"/>
+    </row>
+    <row r="21" spans="5:36" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="57"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="K21" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="L21" s="56" t="s">
+        <v>116</v>
+      </c>
+      <c r="M21" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="U21" s="52"/>
+      <c r="V21" s="52"/>
+      <c r="W21" s="52" t="s">
+        <v>203</v>
+      </c>
+      <c r="X21" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y21" s="52" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z21" s="55" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA21" s="52" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB21" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC21" s="54" t="s">
+        <v>217</v>
+      </c>
+      <c r="AD21" s="56"/>
+      <c r="AE21" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="AF21" s="56"/>
+      <c r="AG21" s="56" t="s">
+        <v>243</v>
+      </c>
+      <c r="AH21" s="56"/>
+      <c r="AI21" s="56"/>
+      <c r="AJ21" s="57"/>
+    </row>
+    <row r="22" spans="5:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="E22" s="70"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="K22" s="54" t="s">
+        <v>86</v>
+      </c>
+      <c r="L22" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="M22" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="57"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="52"/>
+      <c r="V22" s="52"/>
+      <c r="W22" s="52"/>
+      <c r="X22" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y22" s="52"/>
+      <c r="Z22" s="46"/>
+      <c r="AA22" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB22" s="51" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC22" s="54" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD22" s="56"/>
+      <c r="AE22" s="56" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF22" s="56"/>
+      <c r="AG22" s="56" t="s">
+        <v>211</v>
+      </c>
+      <c r="AH22" s="56"/>
+      <c r="AI22" s="56"/>
+      <c r="AJ22" s="57"/>
+    </row>
+    <row r="23" spans="5:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="E23" s="71"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56" t="s">
+        <v>150</v>
+      </c>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="K23" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="57"/>
+      <c r="R23" s="42"/>
+      <c r="S23" s="42"/>
+      <c r="T23" s="61"/>
+      <c r="U23" s="52"/>
+      <c r="V23" s="52"/>
+      <c r="W23" s="52"/>
+      <c r="X23" s="52"/>
+      <c r="Y23" s="52"/>
+      <c r="Z23" s="52"/>
+      <c r="AA23" s="52"/>
+      <c r="AB23" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC23" s="54" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD23" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="AE23" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="AF23" s="56"/>
+      <c r="AG23" s="56"/>
+      <c r="AH23" s="56"/>
+      <c r="AI23" s="56"/>
+      <c r="AJ23" s="57"/>
+    </row>
+    <row r="24" spans="5:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="E24" s="62"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="K24" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="L24" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="M24" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="N24" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="O24" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="P24" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q24" s="57"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="42"/>
+      <c r="T24" s="61"/>
+      <c r="U24" s="52"/>
+      <c r="V24" s="52"/>
+      <c r="W24" s="52"/>
+      <c r="X24" s="52" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y24" s="52" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z24" s="52"/>
+      <c r="AA24" s="52" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB24" s="51" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC24" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD24" s="56"/>
+      <c r="AE24" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF24" s="56"/>
+      <c r="AG24" s="56"/>
+      <c r="AH24" s="56"/>
+      <c r="AI24" s="56"/>
+      <c r="AJ24" s="57"/>
+    </row>
+    <row r="25" spans="5:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" s="71"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="J25" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="K25" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="L25" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="M25" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="N25" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="O25" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="P25" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="61"/>
+      <c r="U25" s="52"/>
+      <c r="V25" s="52"/>
+      <c r="W25" s="52"/>
+      <c r="X25" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y25" s="52" t="s">
+        <v>240</v>
+      </c>
+      <c r="Z25" s="52"/>
+      <c r="AA25" s="52" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB25" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC25" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD25" s="56"/>
+      <c r="AE25" s="56"/>
+      <c r="AF25" s="56"/>
+      <c r="AG25" s="56"/>
+      <c r="AH25" s="56"/>
+      <c r="AI25" s="56"/>
+      <c r="AJ25" s="57"/>
+    </row>
+    <row r="26" spans="5:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="E26" s="69"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" s="56" t="s">
+        <v>194</v>
+      </c>
+      <c r="J26" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="K26" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="L26" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="M26" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="N26" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="O26" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="P26" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q26" s="57"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="42"/>
+      <c r="T26" s="61"/>
+      <c r="U26" s="52"/>
+      <c r="V26" s="52"/>
+      <c r="W26" s="52"/>
+      <c r="X26" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y26" s="52"/>
+      <c r="Z26" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA26" s="52"/>
+      <c r="AB26" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="AC26" s="54" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD26" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="AE26" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF26" s="56"/>
+      <c r="AG26" s="56"/>
+      <c r="AH26" s="56"/>
+      <c r="AI26" s="56"/>
+      <c r="AJ26" s="57"/>
+    </row>
+    <row r="27" spans="5:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="E27" s="57"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="K27" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="57"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="61"/>
+      <c r="U27" s="52"/>
+      <c r="V27" s="52"/>
+      <c r="W27" s="52"/>
+      <c r="X27" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="52"/>
+      <c r="AA27" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB27" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC27" s="54" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD27" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE27" s="56"/>
+      <c r="AF27" s="56"/>
+      <c r="AG27" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH27" s="56"/>
+      <c r="AI27" s="56"/>
+      <c r="AJ27" s="57"/>
+    </row>
+    <row r="28" spans="5:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="E28" s="95" t="s">
+        <v>279</v>
+      </c>
+      <c r="F28" s="96"/>
+      <c r="G28" s="96"/>
+      <c r="H28" s="96"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="96"/>
+      <c r="K28" s="96"/>
+      <c r="L28" s="96"/>
+      <c r="M28" s="96"/>
+      <c r="N28" s="96"/>
+      <c r="O28" s="96"/>
+      <c r="P28" s="96"/>
+      <c r="Q28" s="96"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="61"/>
+      <c r="U28" s="52"/>
+      <c r="V28" s="52"/>
+      <c r="W28" s="52"/>
+      <c r="X28" s="52"/>
+      <c r="Y28" s="52"/>
+      <c r="Z28" s="52"/>
+      <c r="AA28" s="52"/>
+      <c r="AB28" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC28" s="54" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD28" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="AE28" s="56"/>
+      <c r="AF28" s="56"/>
+      <c r="AG28" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH28" s="56"/>
+      <c r="AI28" s="56"/>
+      <c r="AJ28" s="57"/>
+    </row>
+    <row r="29" spans="5:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="42"/>
+      <c r="T29" s="61"/>
+      <c r="U29" s="52"/>
+      <c r="V29" s="52"/>
+      <c r="W29" s="52"/>
+      <c r="X29" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y29" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z29" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA29" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB29" s="51" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC29" s="54" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD29" s="56"/>
+      <c r="AE29" s="56"/>
+      <c r="AF29" s="56"/>
+      <c r="AG29" s="56"/>
+      <c r="AH29" s="56"/>
+      <c r="AI29" s="56"/>
+      <c r="AJ29" s="57"/>
+    </row>
+    <row r="30" spans="5:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="42"/>
+      <c r="Q30" s="42"/>
+      <c r="R30" s="42"/>
+      <c r="S30" s="42"/>
+      <c r="T30" s="61"/>
+      <c r="U30" s="52"/>
+      <c r="V30" s="52" t="s">
+        <v>263</v>
+      </c>
+      <c r="W30" s="52"/>
+      <c r="X30" s="52" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y30" s="52"/>
+      <c r="Z30" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA30" s="52" t="s">
+        <v>244</v>
+      </c>
+      <c r="AB30" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC30" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD30" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE30" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF30" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="AG30" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="AH30" s="56"/>
+      <c r="AI30" s="56" t="s">
+        <v>260</v>
+      </c>
+      <c r="AJ30" s="57"/>
+    </row>
+    <row r="31" spans="5:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="42"/>
+      <c r="Q31" s="42"/>
+      <c r="R31" s="42"/>
+      <c r="S31" s="42"/>
+      <c r="T31" s="57"/>
+      <c r="U31" s="56"/>
+      <c r="V31" s="56"/>
+      <c r="W31" s="56"/>
+      <c r="X31" s="56"/>
+      <c r="Y31" s="56"/>
+      <c r="Z31" s="56" t="s">
+        <v>258</v>
+      </c>
+      <c r="AA31" s="56"/>
+      <c r="AB31" s="51" t="s">
+        <v>236</v>
+      </c>
+      <c r="AC31" s="54" t="s">
+        <v>226</v>
+      </c>
+      <c r="AD31" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE31" s="56"/>
+      <c r="AF31" s="56" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG31" s="56"/>
+      <c r="AH31" s="56"/>
+      <c r="AI31" s="56" t="s">
+        <v>261</v>
+      </c>
+      <c r="AJ31" s="57"/>
+    </row>
+    <row r="32" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E32" s="1"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="95" t="s">
+        <v>281</v>
+      </c>
+      <c r="U32" s="96"/>
+      <c r="V32" s="96"/>
+      <c r="W32" s="96"/>
+      <c r="X32" s="96"/>
+      <c r="Y32" s="96"/>
+      <c r="Z32" s="96"/>
+      <c r="AA32" s="96"/>
+      <c r="AB32" s="96"/>
+      <c r="AC32" s="96"/>
+      <c r="AD32" s="96"/>
+      <c r="AE32" s="96"/>
+      <c r="AF32" s="96"/>
+      <c r="AG32" s="96"/>
+      <c r="AH32" s="96"/>
+      <c r="AI32" s="96"/>
+      <c r="AJ32" s="96"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E3:Q3"/>
+    <mergeCell ref="T3:AJ3"/>
+    <mergeCell ref="E28:Q28"/>
+    <mergeCell ref="T32:AJ32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B245FEE-59D5-4395-9E5E-1CEE046AA18E}">
   <dimension ref="C3:V25"/>
   <sheetViews>
@@ -4863,32 +6574,32 @@
   <sheetData>
     <row r="3" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="123" t="s">
+      <c r="C4" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="125"/>
-      <c r="H4" s="126" t="s">
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="117"/>
+      <c r="H4" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="127"/>
-      <c r="J4" s="128"/>
-      <c r="L4" s="115" t="s">
+      <c r="I4" s="119"/>
+      <c r="J4" s="120"/>
+      <c r="L4" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="116"/>
-      <c r="N4" s="117"/>
-      <c r="P4" s="115" t="s">
+      <c r="M4" s="108"/>
+      <c r="N4" s="109"/>
+      <c r="P4" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="116"/>
-      <c r="R4" s="117"/>
-      <c r="T4" s="115" t="s">
+      <c r="Q4" s="108"/>
+      <c r="R4" s="109"/>
+      <c r="T4" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="U4" s="116"/>
-      <c r="V4" s="117"/>
+      <c r="U4" s="108"/>
+      <c r="V4" s="109"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="31" t="s">
@@ -4941,7 +6652,7 @@
       </c>
     </row>
     <row r="6" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C6" s="120" t="s">
+      <c r="C6" s="112" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="22">
@@ -4953,7 +6664,7 @@
       <c r="F6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="120" t="s">
+      <c r="H6" s="112" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="26">
@@ -4962,7 +6673,7 @@
       <c r="J6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="129" t="s">
+      <c r="L6" s="121" t="s">
         <v>3</v>
       </c>
       <c r="M6" s="22">
@@ -4971,7 +6682,7 @@
       <c r="N6" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="69" t="s">
+      <c r="P6" s="75" t="s">
         <v>6</v>
       </c>
       <c r="Q6" s="25">
@@ -4989,7 +6700,7 @@
       <c r="V6" s="6"/>
     </row>
     <row r="7" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="121"/>
+      <c r="C7" s="113"/>
       <c r="D7" s="22">
         <v>3</v>
       </c>
@@ -4999,28 +6710,28 @@
       <c r="F7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="121"/>
+      <c r="H7" s="113"/>
       <c r="I7" s="22">
         <v>11</v>
       </c>
       <c r="J7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="130"/>
+      <c r="L7" s="122"/>
       <c r="M7" s="24">
         <v>15</v>
       </c>
       <c r="N7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="P7" s="70"/>
+      <c r="P7" s="76"/>
       <c r="Q7" s="12">
         <v>9</v>
       </c>
       <c r="R7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="T7" s="118" t="s">
+      <c r="T7" s="110" t="s">
         <v>3</v>
       </c>
       <c r="U7" s="26">
@@ -5029,7 +6740,7 @@
       <c r="V7" s="29"/>
     </row>
     <row r="8" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="129"/>
+      <c r="C8" s="121"/>
       <c r="D8" s="22">
         <v>4</v>
       </c>
@@ -5039,31 +6750,31 @@
       <c r="F8" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="122"/>
+      <c r="H8" s="114"/>
       <c r="I8" s="24">
         <v>12</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="98" t="s">
+      <c r="L8" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="M8" s="99"/>
-      <c r="N8" s="100"/>
-      <c r="P8" s="98" t="s">
+      <c r="M8" s="124"/>
+      <c r="N8" s="125"/>
+      <c r="P8" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="99"/>
-      <c r="R8" s="100"/>
-      <c r="T8" s="76"/>
+      <c r="Q8" s="124"/>
+      <c r="R8" s="125"/>
+      <c r="T8" s="82"/>
       <c r="U8" s="34">
         <v>13</v>
       </c>
       <c r="V8" s="35"/>
     </row>
     <row r="9" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C9" s="121" t="s">
+      <c r="C9" s="113" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="25">
@@ -5075,29 +6786,29 @@
       <c r="F9" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="101" t="s">
+      <c r="H9" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="102"/>
-      <c r="J9" s="103"/>
-      <c r="L9" s="93" t="s">
+      <c r="I9" s="127"/>
+      <c r="J9" s="128"/>
+      <c r="L9" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="94"/>
-      <c r="N9" s="95"/>
-      <c r="P9" s="93" t="s">
+      <c r="M9" s="103"/>
+      <c r="N9" s="104"/>
+      <c r="P9" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="95"/>
-      <c r="T9" s="119"/>
+      <c r="Q9" s="103"/>
+      <c r="R9" s="104"/>
+      <c r="T9" s="111"/>
       <c r="U9" s="27">
         <v>15</v>
       </c>
       <c r="V9" s="33"/>
     </row>
     <row r="10" spans="3:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="121"/>
+      <c r="C10" s="113"/>
       <c r="D10" s="28">
         <v>9</v>
       </c>
@@ -5107,18 +6818,18 @@
       <c r="F10" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="104" t="s">
+      <c r="H10" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="105"/>
-      <c r="J10" s="106"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="94"/>
-      <c r="N10" s="95"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="94"/>
-      <c r="R10" s="95"/>
-      <c r="T10" s="118" t="s">
+      <c r="I10" s="130"/>
+      <c r="J10" s="131"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="103"/>
+      <c r="N10" s="104"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="104"/>
+      <c r="T10" s="110" t="s">
         <v>4</v>
       </c>
       <c r="U10" s="26">
@@ -5127,7 +6838,7 @@
       <c r="V10" s="29"/>
     </row>
     <row r="11" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="112" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="22">
@@ -5139,23 +6850,23 @@
       <c r="F11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="93"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="108"/>
-      <c r="L11" s="76"/>
-      <c r="M11" s="94"/>
-      <c r="N11" s="95"/>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="94"/>
-      <c r="R11" s="95"/>
-      <c r="T11" s="72"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="132"/>
+      <c r="J11" s="133"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="104"/>
+      <c r="P11" s="82"/>
+      <c r="Q11" s="103"/>
+      <c r="R11" s="104"/>
+      <c r="T11" s="78"/>
       <c r="U11" s="36">
         <v>7</v>
       </c>
       <c r="V11" s="37"/>
     </row>
     <row r="12" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C12" s="121"/>
+      <c r="C12" s="113"/>
       <c r="D12" s="22">
         <v>12</v>
       </c>
@@ -5165,18 +6876,18 @@
       <c r="F12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="93"/>
-      <c r="I12" s="107"/>
-      <c r="J12" s="108"/>
-      <c r="L12" s="76"/>
-      <c r="M12" s="94"/>
-      <c r="N12" s="95"/>
-      <c r="P12" s="76"/>
-      <c r="Q12" s="94"/>
-      <c r="R12" s="95"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="132"/>
+      <c r="J12" s="133"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="103"/>
+      <c r="N12" s="104"/>
+      <c r="P12" s="82"/>
+      <c r="Q12" s="103"/>
+      <c r="R12" s="104"/>
     </row>
     <row r="13" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="122"/>
+      <c r="C13" s="114"/>
       <c r="D13" s="24">
         <v>13</v>
       </c>
@@ -5186,151 +6897,162 @@
       <c r="F13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="93"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="108"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="95"/>
-      <c r="P13" s="76"/>
-      <c r="Q13" s="94"/>
-      <c r="R13" s="95"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="132"/>
+      <c r="J13" s="133"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="104"/>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="104"/>
     </row>
     <row r="14" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C14" s="112" t="s">
+      <c r="C14" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="113"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="114"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="107"/>
-      <c r="J14" s="108"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="94"/>
-      <c r="N14" s="95"/>
-      <c r="P14" s="76"/>
-      <c r="Q14" s="94"/>
-      <c r="R14" s="95"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="101"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="132"/>
+      <c r="J14" s="133"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="103"/>
+      <c r="N14" s="104"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="103"/>
+      <c r="R14" s="104"/>
     </row>
     <row r="15" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C15" s="93" t="s">
+      <c r="C15" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="107"/>
-      <c r="J15" s="108"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="95"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="94"/>
-      <c r="R15" s="95"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="103"/>
+      <c r="F15" s="104"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="132"/>
+      <c r="J15" s="133"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="104"/>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="103"/>
+      <c r="R15" s="104"/>
     </row>
     <row r="16" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="72"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="97"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="107"/>
-      <c r="J16" s="108"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="96"/>
-      <c r="N16" s="97"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="96"/>
-      <c r="R16" s="97"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="106"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="132"/>
+      <c r="J16" s="133"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="105"/>
+      <c r="N16" s="106"/>
+      <c r="P16" s="78"/>
+      <c r="Q16" s="105"/>
+      <c r="R16" s="106"/>
     </row>
     <row r="17" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H17" s="93"/>
-      <c r="I17" s="107"/>
-      <c r="J17" s="108"/>
-      <c r="L17" s="112" t="s">
+      <c r="H17" s="102"/>
+      <c r="I17" s="132"/>
+      <c r="J17" s="133"/>
+      <c r="L17" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="M17" s="113"/>
-      <c r="N17" s="114"/>
-      <c r="P17" s="112" t="s">
+      <c r="M17" s="100"/>
+      <c r="N17" s="101"/>
+      <c r="P17" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="Q17" s="113"/>
-      <c r="R17" s="114"/>
+      <c r="Q17" s="100"/>
+      <c r="R17" s="101"/>
     </row>
     <row r="18" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H18" s="93"/>
-      <c r="I18" s="107"/>
-      <c r="J18" s="108"/>
-      <c r="L18" s="93" t="s">
+      <c r="H18" s="102"/>
+      <c r="I18" s="132"/>
+      <c r="J18" s="133"/>
+      <c r="L18" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="M18" s="94"/>
-      <c r="N18" s="95"/>
-      <c r="P18" s="93" t="s">
+      <c r="M18" s="103"/>
+      <c r="N18" s="104"/>
+      <c r="P18" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="Q18" s="94"/>
-      <c r="R18" s="95"/>
+      <c r="Q18" s="103"/>
+      <c r="R18" s="104"/>
     </row>
     <row r="19" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H19" s="109"/>
-      <c r="I19" s="110"/>
-      <c r="J19" s="111"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="94"/>
-      <c r="N19" s="95"/>
-      <c r="P19" s="72"/>
-      <c r="Q19" s="96"/>
-      <c r="R19" s="97"/>
+      <c r="H19" s="134"/>
+      <c r="I19" s="135"/>
+      <c r="J19" s="136"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="103"/>
+      <c r="N19" s="104"/>
+      <c r="P19" s="78"/>
+      <c r="Q19" s="105"/>
+      <c r="R19" s="106"/>
     </row>
     <row r="20" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H20" s="112" t="s">
+      <c r="H20" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="113"/>
-      <c r="J20" s="114"/>
-      <c r="L20" s="76"/>
-      <c r="M20" s="94"/>
-      <c r="N20" s="95"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="101"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="103"/>
+      <c r="N20" s="104"/>
     </row>
     <row r="21" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H21" s="93" t="s">
+      <c r="H21" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="94"/>
-      <c r="J21" s="95"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="94"/>
-      <c r="N21" s="95"/>
+      <c r="I21" s="103"/>
+      <c r="J21" s="104"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="103"/>
+      <c r="N21" s="104"/>
     </row>
     <row r="22" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H22" s="76"/>
-      <c r="I22" s="94"/>
-      <c r="J22" s="95"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="97"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="103"/>
+      <c r="J22" s="104"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="106"/>
     </row>
     <row r="23" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H23" s="76"/>
-      <c r="I23" s="94"/>
-      <c r="J23" s="95"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="103"/>
+      <c r="J23" s="104"/>
     </row>
     <row r="24" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H24" s="76"/>
-      <c r="I24" s="94"/>
-      <c r="J24" s="95"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="103"/>
+      <c r="J24" s="104"/>
     </row>
     <row r="25" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H25" s="72"/>
-      <c r="I25" s="96"/>
-      <c r="J25" s="97"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="105"/>
+      <c r="J25" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="L9:N16"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R16"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J19"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="L18:N22"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J25"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C15:F16"/>
     <mergeCell ref="T4:V4"/>
@@ -5347,17 +7069,6 @@
     <mergeCell ref="P6:P7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N16"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R16"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J19"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L18:N22"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PID + CAlimentacao + PCB(Shield)
</commit_message>
<xml_diff>
--- a/04Code/Perifericos.xlsx
+++ b/04Code/Perifericos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02Sem\LPI\DWR-19\04Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DWR-19\04Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444109BA-373B-4664-8E19-FFF8A0FD075D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B05B700-B48F-49F1-BD28-EDEF00EEFAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-890" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinos Usados" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="297">
   <si>
     <t>Porto</t>
   </si>
@@ -946,6 +946,9 @@
   </si>
   <si>
     <t>ADC3/10</t>
+  </si>
+  <si>
+    <t>Buffer</t>
   </si>
 </sst>
 </file>
@@ -1921,6 +1924,15 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1936,6 +1948,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1977,63 +2037,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4878,8 +4881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FE4C32-C97D-45A9-AB28-ECC31E431526}">
   <dimension ref="A1:AJ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5744,7 +5747,9 @@
       <c r="Q17" s="57"/>
       <c r="R17" s="42"/>
       <c r="S17" s="42"/>
-      <c r="T17" s="57"/>
+      <c r="T17" s="57" t="s">
+        <v>296</v>
+      </c>
       <c r="U17" s="56"/>
       <c r="V17" s="56"/>
       <c r="W17" s="56"/>
@@ -5796,7 +5801,9 @@
       <c r="Q18" s="59"/>
       <c r="R18" s="42"/>
       <c r="S18" s="42"/>
-      <c r="T18" s="61"/>
+      <c r="T18" s="61" t="s">
+        <v>296</v>
+      </c>
       <c r="U18" s="52"/>
       <c r="V18" s="52" t="s">
         <v>262</v>
@@ -6595,32 +6602,32 @@
   <sheetData>
     <row r="3" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="129" t="s">
+      <c r="C4" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
-      <c r="H4" s="132" t="s">
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="117"/>
+      <c r="H4" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="133"/>
-      <c r="J4" s="134"/>
-      <c r="L4" s="121" t="s">
+      <c r="I4" s="119"/>
+      <c r="J4" s="120"/>
+      <c r="L4" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="122"/>
-      <c r="N4" s="123"/>
-      <c r="P4" s="121" t="s">
+      <c r="M4" s="108"/>
+      <c r="N4" s="109"/>
+      <c r="P4" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="123"/>
-      <c r="T4" s="121" t="s">
+      <c r="Q4" s="108"/>
+      <c r="R4" s="109"/>
+      <c r="T4" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="U4" s="122"/>
-      <c r="V4" s="123"/>
+      <c r="U4" s="108"/>
+      <c r="V4" s="109"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="31" t="s">
@@ -6673,7 +6680,7 @@
       </c>
     </row>
     <row r="6" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C6" s="126" t="s">
+      <c r="C6" s="112" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="22">
@@ -6685,7 +6692,7 @@
       <c r="F6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="126" t="s">
+      <c r="H6" s="112" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="26">
@@ -6694,7 +6701,7 @@
       <c r="J6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="135" t="s">
+      <c r="L6" s="121" t="s">
         <v>3</v>
       </c>
       <c r="M6" s="22">
@@ -6721,7 +6728,7 @@
       <c r="V6" s="6"/>
     </row>
     <row r="7" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="127"/>
+      <c r="C7" s="113"/>
       <c r="D7" s="22">
         <v>3</v>
       </c>
@@ -6731,14 +6738,14 @@
       <c r="F7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="127"/>
+      <c r="H7" s="113"/>
       <c r="I7" s="22">
         <v>11</v>
       </c>
       <c r="J7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="136"/>
+      <c r="L7" s="122"/>
       <c r="M7" s="24">
         <v>15</v>
       </c>
@@ -6752,7 +6759,7 @@
       <c r="R7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="T7" s="124" t="s">
+      <c r="T7" s="110" t="s">
         <v>3</v>
       </c>
       <c r="U7" s="26">
@@ -6761,7 +6768,7 @@
       <c r="V7" s="29"/>
     </row>
     <row r="8" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="135"/>
+      <c r="C8" s="121"/>
       <c r="D8" s="22">
         <v>4</v>
       </c>
@@ -6771,23 +6778,23 @@
       <c r="F8" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="128"/>
+      <c r="H8" s="114"/>
       <c r="I8" s="24">
         <v>12</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="104" t="s">
+      <c r="L8" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="M8" s="105"/>
-      <c r="N8" s="106"/>
-      <c r="P8" s="104" t="s">
+      <c r="M8" s="124"/>
+      <c r="N8" s="125"/>
+      <c r="P8" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="105"/>
-      <c r="R8" s="106"/>
+      <c r="Q8" s="124"/>
+      <c r="R8" s="125"/>
       <c r="T8" s="82"/>
       <c r="U8" s="34">
         <v>13</v>
@@ -6795,7 +6802,7 @@
       <c r="V8" s="35"/>
     </row>
     <row r="9" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C9" s="127" t="s">
+      <c r="C9" s="113" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="25">
@@ -6807,29 +6814,29 @@
       <c r="F9" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="107" t="s">
+      <c r="H9" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="108"/>
-      <c r="J9" s="109"/>
-      <c r="L9" s="99" t="s">
+      <c r="I9" s="127"/>
+      <c r="J9" s="128"/>
+      <c r="L9" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="100"/>
-      <c r="N9" s="101"/>
-      <c r="P9" s="99" t="s">
+      <c r="M9" s="103"/>
+      <c r="N9" s="104"/>
+      <c r="P9" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="Q9" s="100"/>
-      <c r="R9" s="101"/>
-      <c r="T9" s="125"/>
+      <c r="Q9" s="103"/>
+      <c r="R9" s="104"/>
+      <c r="T9" s="111"/>
       <c r="U9" s="27">
         <v>15</v>
       </c>
       <c r="V9" s="33"/>
     </row>
     <row r="10" spans="3:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="127"/>
+      <c r="C10" s="113"/>
       <c r="D10" s="28">
         <v>9</v>
       </c>
@@ -6839,18 +6846,18 @@
       <c r="F10" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="110" t="s">
+      <c r="H10" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="111"/>
-      <c r="J10" s="112"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="131"/>
       <c r="L10" s="82"/>
-      <c r="M10" s="100"/>
-      <c r="N10" s="101"/>
+      <c r="M10" s="103"/>
+      <c r="N10" s="104"/>
       <c r="P10" s="82"/>
-      <c r="Q10" s="100"/>
-      <c r="R10" s="101"/>
-      <c r="T10" s="124" t="s">
+      <c r="Q10" s="103"/>
+      <c r="R10" s="104"/>
+      <c r="T10" s="110" t="s">
         <v>4</v>
       </c>
       <c r="U10" s="26">
@@ -6859,7 +6866,7 @@
       <c r="V10" s="29"/>
     </row>
     <row r="11" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="126" t="s">
+      <c r="C11" s="112" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="22">
@@ -6871,15 +6878,15 @@
       <c r="F11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="99"/>
-      <c r="I11" s="113"/>
-      <c r="J11" s="114"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="132"/>
+      <c r="J11" s="133"/>
       <c r="L11" s="82"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="101"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="104"/>
       <c r="P11" s="82"/>
-      <c r="Q11" s="100"/>
-      <c r="R11" s="101"/>
+      <c r="Q11" s="103"/>
+      <c r="R11" s="104"/>
       <c r="T11" s="78"/>
       <c r="U11" s="36">
         <v>7</v>
@@ -6887,7 +6894,7 @@
       <c r="V11" s="37"/>
     </row>
     <row r="12" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C12" s="127"/>
+      <c r="C12" s="113"/>
       <c r="D12" s="22">
         <v>12</v>
       </c>
@@ -6897,18 +6904,18 @@
       <c r="F12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="99"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="114"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="132"/>
+      <c r="J12" s="133"/>
       <c r="L12" s="82"/>
-      <c r="M12" s="100"/>
-      <c r="N12" s="101"/>
+      <c r="M12" s="103"/>
+      <c r="N12" s="104"/>
       <c r="P12" s="82"/>
-      <c r="Q12" s="100"/>
-      <c r="R12" s="101"/>
+      <c r="Q12" s="103"/>
+      <c r="R12" s="104"/>
     </row>
     <row r="13" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="128"/>
+      <c r="C13" s="114"/>
       <c r="D13" s="24">
         <v>13</v>
       </c>
@@ -6918,151 +6925,162 @@
       <c r="F13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="99"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="114"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="132"/>
+      <c r="J13" s="133"/>
       <c r="L13" s="82"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="101"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="104"/>
       <c r="P13" s="82"/>
-      <c r="Q13" s="100"/>
-      <c r="R13" s="101"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="104"/>
     </row>
     <row r="14" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C14" s="118" t="s">
+      <c r="C14" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="120"/>
-      <c r="H14" s="99"/>
-      <c r="I14" s="113"/>
-      <c r="J14" s="114"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="101"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="132"/>
+      <c r="J14" s="133"/>
       <c r="L14" s="82"/>
-      <c r="M14" s="100"/>
-      <c r="N14" s="101"/>
+      <c r="M14" s="103"/>
+      <c r="N14" s="104"/>
       <c r="P14" s="82"/>
-      <c r="Q14" s="100"/>
-      <c r="R14" s="101"/>
+      <c r="Q14" s="103"/>
+      <c r="R14" s="104"/>
     </row>
     <row r="15" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C15" s="99" t="s">
+      <c r="C15" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="100"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="101"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="113"/>
-      <c r="J15" s="114"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="103"/>
+      <c r="F15" s="104"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="132"/>
+      <c r="J15" s="133"/>
       <c r="L15" s="82"/>
-      <c r="M15" s="100"/>
-      <c r="N15" s="101"/>
+      <c r="M15" s="103"/>
+      <c r="N15" s="104"/>
       <c r="P15" s="82"/>
-      <c r="Q15" s="100"/>
-      <c r="R15" s="101"/>
+      <c r="Q15" s="103"/>
+      <c r="R15" s="104"/>
     </row>
     <row r="16" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="78"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="103"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="113"/>
-      <c r="J16" s="114"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="106"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="132"/>
+      <c r="J16" s="133"/>
       <c r="L16" s="78"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="103"/>
+      <c r="M16" s="105"/>
+      <c r="N16" s="106"/>
       <c r="P16" s="78"/>
-      <c r="Q16" s="102"/>
-      <c r="R16" s="103"/>
+      <c r="Q16" s="105"/>
+      <c r="R16" s="106"/>
     </row>
     <row r="17" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H17" s="99"/>
-      <c r="I17" s="113"/>
-      <c r="J17" s="114"/>
-      <c r="L17" s="118" t="s">
+      <c r="H17" s="102"/>
+      <c r="I17" s="132"/>
+      <c r="J17" s="133"/>
+      <c r="L17" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="M17" s="119"/>
-      <c r="N17" s="120"/>
-      <c r="P17" s="118" t="s">
+      <c r="M17" s="100"/>
+      <c r="N17" s="101"/>
+      <c r="P17" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="Q17" s="119"/>
-      <c r="R17" s="120"/>
+      <c r="Q17" s="100"/>
+      <c r="R17" s="101"/>
     </row>
     <row r="18" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H18" s="99"/>
-      <c r="I18" s="113"/>
-      <c r="J18" s="114"/>
-      <c r="L18" s="99" t="s">
+      <c r="H18" s="102"/>
+      <c r="I18" s="132"/>
+      <c r="J18" s="133"/>
+      <c r="L18" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="M18" s="100"/>
-      <c r="N18" s="101"/>
-      <c r="P18" s="99" t="s">
+      <c r="M18" s="103"/>
+      <c r="N18" s="104"/>
+      <c r="P18" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="Q18" s="100"/>
-      <c r="R18" s="101"/>
+      <c r="Q18" s="103"/>
+      <c r="R18" s="104"/>
     </row>
     <row r="19" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H19" s="115"/>
-      <c r="I19" s="116"/>
-      <c r="J19" s="117"/>
+      <c r="H19" s="134"/>
+      <c r="I19" s="135"/>
+      <c r="J19" s="136"/>
       <c r="L19" s="82"/>
-      <c r="M19" s="100"/>
-      <c r="N19" s="101"/>
+      <c r="M19" s="103"/>
+      <c r="N19" s="104"/>
       <c r="P19" s="78"/>
-      <c r="Q19" s="102"/>
-      <c r="R19" s="103"/>
+      <c r="Q19" s="105"/>
+      <c r="R19" s="106"/>
     </row>
     <row r="20" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H20" s="118" t="s">
+      <c r="H20" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="I20" s="119"/>
-      <c r="J20" s="120"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="101"/>
       <c r="L20" s="82"/>
-      <c r="M20" s="100"/>
-      <c r="N20" s="101"/>
+      <c r="M20" s="103"/>
+      <c r="N20" s="104"/>
     </row>
     <row r="21" spans="8:18" x14ac:dyDescent="0.25">
-      <c r="H21" s="99" t="s">
+      <c r="H21" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="100"/>
-      <c r="J21" s="101"/>
+      <c r="I21" s="103"/>
+      <c r="J21" s="104"/>
       <c r="L21" s="82"/>
-      <c r="M21" s="100"/>
-      <c r="N21" s="101"/>
+      <c r="M21" s="103"/>
+      <c r="N21" s="104"/>
     </row>
     <row r="22" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H22" s="82"/>
-      <c r="I22" s="100"/>
-      <c r="J22" s="101"/>
+      <c r="I22" s="103"/>
+      <c r="J22" s="104"/>
       <c r="L22" s="78"/>
-      <c r="M22" s="102"/>
-      <c r="N22" s="103"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="106"/>
     </row>
     <row r="23" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H23" s="82"/>
-      <c r="I23" s="100"/>
-      <c r="J23" s="101"/>
+      <c r="I23" s="103"/>
+      <c r="J23" s="104"/>
     </row>
     <row r="24" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H24" s="82"/>
-      <c r="I24" s="100"/>
-      <c r="J24" s="101"/>
+      <c r="I24" s="103"/>
+      <c r="J24" s="104"/>
     </row>
     <row r="25" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H25" s="78"/>
-      <c r="I25" s="102"/>
-      <c r="J25" s="103"/>
+      <c r="I25" s="105"/>
+      <c r="J25" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="L9:N16"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:R16"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J19"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="L18:N22"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J25"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C15:F16"/>
     <mergeCell ref="T4:V4"/>
@@ -7079,17 +7097,6 @@
     <mergeCell ref="P6:P7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N16"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:R16"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J19"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L18:N22"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>